<commit_message>
update input and readme
</commit_message>
<xml_diff>
--- a/FDS/test_output/Design_results.xlsx
+++ b/FDS/test_output/Design_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,36 +480,36 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dxs_sub_933_C_T_sub</t>
+          <t>b0003</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>GTAAGCTCCTGGGGCTTCAC</t>
+          <t>ACTTACGTGTCTGCGGTGTT</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>GGCCTCGTGATACGCCTATTACCGAAAAGTAGCGGCGGTTT</t>
+          <t>GGCCTCGTGATACGCCTATTGTCAGACTCCTAACTTCCATGAGA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>GTAAGCTCCTGGGGCTTCACTCGTTTGCCGCCTTCCTGCAACTCGAATTATTTAGAGTCTATGAATAATTTCTTAAGCATAGCAGGAGTGGAGTAGGGATTATGCCAGCCAGGCCTTGATTTTGGCTTCCATACCAGCGGCATCGAGGCCGAGTTCGGCGCGCATTTCTTCCTGAGTTCCTTGCGGAATAAAGAAGTCCGGCAGGCCAATGTTCAGCACGGGTACTGGTTTACGATGGGCCATCAGCACTTCGTTCACGCCGCTGCCTGCGCCGCCCATAATGGCGTTTTCTTCTACGGTGACCAGCGCTTCATGGCTGGCGGCCATTTCCAGAATTAACGCTTCATCAAGCGGTTTCACAAAACGCATATCGACCAGCGTGGCGTTCAGCGATTCGGCGACTTTCGCCGCTTCTGGCATCAGCGTACCAAAGTTAAGGATCGCCAGTTTCTCGCCACGACGCTTCACAATGCCTTTGCCAATTGGTAGTTTTTCCAGCGGCGTCAGTTCCACGCCGACCGCGTTGCCACGCGGGTAGCGCACCGCTGACGGGCCATCGTTATAGTGATAGCCGGTATAGAGCATCTGGCGACATTCGTTTTCATCGCTCGGGGTCATAATGACCATTTCCGGTATGCAGCGCAGGTAAGAGAGATCAAAAGCACCCTGATGGGTTTGACCGTCAGCACCAACAATGCCCGCGCGGTCGATGGCGAACAGGACCGGAAGCTTTTGAATCGCCACGTCATGCAGCACCTGATCATAGGCGCGTTGCAGGAAAGTGGAGTAAATCGCGACAATGGGTTTGTACCCACCAATCGCCAGACCCGCAGCAAAGGTCACCGCGTGTTGCTCGGCAATTGCCACGTCGAAGTAGCGATCCGGGAATTTACGTGAAAACTCGACCATGCCGGAACCTTCACGCATCGCCGGAGTAATCGCCATCAGCTTGTTGTCTTTCGCTGCCGTTTCGCACAACCAGTCGCCAAAGATTTTTGAATAGCTCGGCAAACCGCCGCTACTTTTCGG</t>
+          <t>ACTTACGTGTCTGCGGTGTTGCCAACTCGAAGGCTCTGCTCACCAATGTACATGGCCTTAATCTGGAAAACTGGCAGGAAGAACTGGCGCAAGCCAAAGAGCCGTTTAATCTCGGGCGCTTAATTCGCCTCGTGAAAGAATATCATCTGCTGAACCCGGTCATTGTTGACTGCACTTCCAGCCAGGCAGTGGCGGATCAATATGCCGACTTCCTGCGCGAAGGTTTCCACGTTGTCACGCCGAACAAAAAGGCCAACACCTCGTCGATGGATTACTACCATCAGTTGCGTTATGCGGCGGAAAAATCGCGGCGTAAATTCCTCTATGACACCAACGTTGGGGCTGGATTACCGGTTATTGAGAACCTGCAAAATCTGCTCAATGCAGGTGATGAATTGATGAAGTTCTCCGGCATTCTTTCTGGTTCGCTTTCTTATATCTTCGGCAAGTTAGACGAAGGCATGAGTTTCTCCGAGGCGACCACGCTGGCGCGGGAAATGGGTTATACCGAACCGGACCCGCGAGATGATCTTTCTGGTATGGATGTGGCGCGTAAACTATTGATTCTCGCTCGTGAAACGGGACGTGAACTGGAGCTGGCGGATATTGAAATTGAACCTGTGCTGCCCGCAGAGTTTAACGCCGAGGGTGATGTTGCCGCTTTTATGGCGAATCTGTCACAACTCGACGATCTCTTTGCCGCGCGCGTGGCGAAGGCCCGTGATGAAGGAAAAGTTTTGCGCTATGTTGGCAATATTGATGAAGATGGCGTCTGCCGCGTGAAGATTGCCGAAGTGGATGGTAATGATCCGCTGTTCAAAGTGAAAAATGGCGAAAACGCCCTGGCCTTCTATAGCCACTATTATCAGCCGCTGCCGTTGGTACTGCGCGGATATGGTGCGGGCAATGACGTTACAGCTGCCGGTGTCTTTGCTGATCTGCTACGTACCCTCTCATGGAAGTTAGGAGTCTGAC</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>CAAAGTCGGGAAACGCGAAGGTCGGTTTTTCCTAAGGGGTTGTATTGCATGCTGCCACTCCTGCTATACTCGTCATACTTCAAGTTGCATGTGCTGCGGCTGCATTCGTTCACCCCAGTCACTTACTTATGTAAGCTCCTGGGGCTTCACTCGTTTGCCGCCTTCCTGCAACTCGAATTATTTAGAGTCTATGAATAATTTCTTAAGCATAGCAGGAGTGGAGTAGGGATTATGCCAGCCAGGCCTTGATTTTGGCTTCCATACCAGCGGCATCGAGGCCGAGTTCGGCGCGCATTTCTTCCTGAGTTCCTTGCGGAATAAAGAAGTCCGGCAGGCCAATGTTCAGCACGGGTACTGGTTTACGATGGGCCATCAGCACTTCGTTCACGCCGCTGCCTGCGCCGCCCATAATGGCGTTTTCTTCTACGGTGACCAGCGCTTCATGGCTGGCGGCCATTTCCAGAATTAACGCTTCATCAAGCGGTTTCACAAAACGCATATCGACCAGCGTGGCGTTCAGCGATTCGGCGACTTTCGCCGCTTCTGGCATCAGCGTACCAAAGTTAAGGATCGCCAGTTTCTCGCCACGACGCTTCACAATGCCTTTGCCAATTGGTAGTTTTTCCAGCGGCGTCAGTTCCACGCCGACCGCGTTGCCACGCGGGTAGCGCACCGCTGACGGGCCATCGTTATAGTGATAGCCGGTATAGAGCATCTGGCGACATTCGTTTTCATCGCTCGGGGTCATAATGACCATTTCCGGTATGCAGCGCAGGTAAGAGAGATCAAAAGCACCCTGATGGGTTTGACCGTCAGCACCAACAATGCCCGCGCGGTCGATGGCGAACAGGACCGGAAGCTTTTGAATCGCCACGTCATGCAGCACCTGATCATAGGCGCGTTGCAGGAAAGTGGAGTAAATCGCGACAATGGGTTTGTACCCACCAATCGCCAGACCCGCAGCAAAGGTCACCGCGTGTTGCTCGGCAATTGCCACGTCGAAGTAGCGATCCGGGAATTTACGTGAAAACTCGACCATGCCGGAACCTTCACGCATCGCCGGAGTAATCGCCATCAGCTTGTTGTCTTTCGCTGCCGTTTCGCACAACCAGTCGCCAAAGATTTTTGAATAGCTCGGCAAACCGCCGCTACTTTTCGG</t>
+          <t>GTTACTCATCAGATGCTGTTCAATACCGATCAGGTTATCGAAGTGTTTGTGATTGGCGTCGGTGGCGTTGGCGGTGCGCTGCTGGAGCAACTGAAGCGTCAGCAAAGCTGGCTGAAGAATAAACATATCGACTTACGTGTCTGCGGTGTTGCCAACTCGAAGGCTCTGCTCACCAATGTACATGGCCTTAATCTGGAAAACTGGCAGGAAGAACTGGCGCAAGCCAAAGAGCCGTTTAATCTCGGGCGCTTAATTCGCCTCGTGAAAGAATATCATCTGCTGAACCCGGTCATTGTTGACTGCACTTCCAGCCAGGCAGTGGCGGATCAATATGCCGACTTCCTGCGCGAAGGTTTCCACGTTGTCACGCCGAACAAAAAGGCCAACACCTCGTCGATGGATTACTACCATCAGTTGCGTTATGCGGCGGAAAAATCGCGGCGTAAATTCCTCTATGACACCAACGTTGGGGCTGGATTACCGGTTATTGAGAACCTGCAAAATCTGCTCAATGCAGGTGATGAATTGATGAAGTTCTCCGGCATTCTTTCTGGTTCGCTTTCTTATATCTTCGGCAAGTTAGACGAAGGCATGAGTTTCTCCGAGGCGACCACGCTGGCGCGGGAAATGGGTTATACCGAACCGGACCCGCGAGATGATCTTTCTGGTATGGATGTGGCGCGTAAACTATTGATTCTCGCTCGTGAAACGGGACGTGAACTGGAGCTGGCGGATATTGAAATTGAACCTGTGCTGCCCGCAGAGTTTAACGCCGAGGGTGATGTTGCCGCTTTTATGGCGAATCTGTCACAACTCGACGATCTCTTTGCCGCGCGCGTGGCGAAGGCCCGTGATGAAGGAAAAGTTTTGCGCTATGTTGGCAATATTGATGAAGATGGCGTCTGCCGCGTGAAGATTGCCGAAGTGGATGGTAATGATCCGCTGTTCAAAGTGAAAAATGGCGAAAACGCCCTGGCCTTCTATAGCCACTATTATCAGCCGCTGCCGTTGGTACTGCGCGGATATGGTGCGGGCAATGACGTTACAGCTGCCGGTGTCTTTGCTGATCTGCTACGTACCCTCTCATGGAAGTTAGGAGTCTGAC</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>GTAAGCTCCTGGGGCTTCACTCGTTTGCCGCCTTCCTGCAACTCGAATTATTTAGAGTCTATGAATAATTTCTTAAGCATAGCAGGAGTGGAGTAGGGATTATGCCAGCCAGGCCTTGATTTTGGCTTCCATACCAGCGGCATCGAGGCCGAGTTCGGCGCGCATTTCTTCCTGAGTTCCTTGCGGAATAAAGAAGTCCGGCAGGCCAATGTTCAGCACGGGTACTGGTTTACGATGGGCCATCAGCACTTCGTTCACGCCGCTGCCTGCGCCGCCCATAATGGCGTTTTCTTCTACGGTGACCAGCGCTTCATGGCTGGCGGCCATTTCCAGAATTAACGCTTCATCAAGCGGTTTCACAAAACGCATATCGACCAGCGTGGCGTTCAGCGATTCGGCGACTTTCGCCGCTTCTGGCATCAGCGTACCAAAGTTAAGGATCGCCAGTTTCTCGCCACGACGCTTCACAATGCCTTTGCCAATTGGTAGTTTTTCCAGCGGCGTCAGTTCCACGCCGACCGCGTTGCCACGCGGGTAGCGCACCGCTGACGGGCCATCGTTATAGTGATAGCCGGTATAGAGCATCTGGCGACATTCGTTTTCATCGCTCGGGGTCATAATGACCATTTCCGGTATGCAGCGCAGGTAAGAGAGATCAAAAGCACCCTGATGGGTTTGACCGTCAGCACCAACAATGCCCGCGCGGTCGATGGCGAACAGGACCGGAAGCTTTTGAATCGCCACGTCATGCAGCACCTGATCATAGGCGCGTTGCAGGAAAGTGGAGTAAATCGCGACAATGGGTTTGTACCCACCAATCGCCAGACCCGCAGCAAAGGTCACCGCGTGTTGCTCGGCAATTGCCACGTCGAAGTAGCGATCCGGGAATTTACGTGAAAACTCGACCATGCCGGAACCTTCACGCATCGCCGGAGTAATCGCCATCAGCTTGTTGTCTTTCGCTGCCGTTTCGCACAACCAGTCGCCAAAGATTTTTGAATAGCTCGGCAAACCGCCGCTACTTTTCGGTAATAGGCGTATCACGAGGCC</t>
+          <t>ACTTACGTGTCTGCGGTGTTGCCAACTCGAAGGCTCTGCTCACCAATGTACATGGCCTTAATCTGGAAAACTGGCAGGAAGAACTGGCGCAAGCCAAAGAGCCGTTTAATCTCGGGCGCTTAATTCGCCTCGTGAAAGAATATCATCTGCTGAACCCGGTCATTGTTGACTGCACTTCCAGCCAGGCAGTGGCGGATCAATATGCCGACTTCCTGCGCGAAGGTTTCCACGTTGTCACGCCGAACAAAAAGGCCAACACCTCGTCGATGGATTACTACCATCAGTTGCGTTATGCGGCGGAAAAATCGCGGCGTAAATTCCTCTATGACACCAACGTTGGGGCTGGATTACCGGTTATTGAGAACCTGCAAAATCTGCTCAATGCAGGTGATGAATTGATGAAGTTCTCCGGCATTCTTTCTGGTTCGCTTTCTTATATCTTCGGCAAGTTAGACGAAGGCATGAGTTTCTCCGAGGCGACCACGCTGGCGCGGGAAATGGGTTATACCGAACCGGACCCGCGAGATGATCTTTCTGGTATGGATGTGGCGCGTAAACTATTGATTCTCGCTCGTGAAACGGGACGTGAACTGGAGCTGGCGGATATTGAAATTGAACCTGTGCTGCCCGCAGAGTTTAACGCCGAGGGTGATGTTGCCGCTTTTATGGCGAATCTGTCACAACTCGACGATCTCTTTGCCGCGCGCGTGGCGAAGGCCCGTGATGAAGGAAAAGTTTTGCGCTATGTTGGCAATATTGATGAAGATGGCGTCTGCCGCGTGAAGATTGCCGAAGTGGATGGTAATGATCCGCTGTTCAAAGTGAAAAATGGCGAAAACGCCCTGGCCTTCTATAGCCACTATTATCAGCCGCTGCCGTTGGTACTGCGCGGATATGGTGCGGGCAATGACGTTACAGCTGCCGGTGTCTTTGCTGATCTGCTACGTACCCTCTCATGGAAGTTAGGAGTCTGACAATAGGCGTATCACGAGGCC</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>1050</v>
+        <v>995</v>
       </c>
     </row>
     <row r="3">
@@ -518,36 +518,36 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>tktA_573_12bp_sub</t>
+          <t>b0004</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>AGGTTCTGACGGGAGAGGAT</t>
+          <t>CAATGACGTTACAGCTGCCG</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>GGCCTCGTGATACGCCTATTCATGTCGAGGGATGGTTCACCGACGACACC</t>
+          <t>GGCCTCGTGATACGCCTATTTTAGTTTTCCAGTACTCGTGCG</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>AGGTTCTGACGGGAGAGGATCAGTGCGGTCGGGCCGTCCTGACGCTCAACACCGTATTTCCACGCGACCGCGGATTCAACCTGGTCACACGGACGCCATGTAGACATGTTCGGGGTTACGCGCAGAGAAGCGACCTGCTCAACCGGCTGGTGAGTCGGGCCGTCTTCGCCCAGACCGATGGAGTCGTGGGTGTAAACCATCACCTGACGCTGTTTCATCAGCGCAGCCATACGTACGGCGTTACGTGCGTATTCCACGAACATCAGGAAGGTGGAGGTGTACGGCAGGAAGCCACCGTGCAGGGAGATACCGTTAGCAATCGCGGTCATACCGAACTCGCGAACACCGTAGTGGATGTAGTTACCCGCAGCATCTTCGTTGATTGCTTTAGAACCAGACCACAGGGTCAGGTTAGACGGCGCCAGGTCAGCAGAACCGCCGAGGAATTCCGGCAACAGCGGACCGAACGCTTCGATAGCATTCTGAGACGCTTTACGGCTGGCGATTTTCGCCGGATTAGCCTGCAGTTTAGCGATGAACTCTTTCGCTTTAGCGTCGAAGTCAGACGGCATTTCGCCTTTCATACGGCGGGTAAATTCAGCGGCTTCCTGCGGATAAGCTTTCGCGTAAGCAGCGAATTTCTCGTTCCATGCGGATTCTTTCGCCTGGCCTGCTTCTTTCGCATCCCACTGAGCATAGATTTCAGACGGGATTTCGAACGGCGCATATTTCCAGCCCAGTTGTTCGCGGGTCAGGGCAATTTCAGCGTCGCCCAGCGGCGCACCGTGGGAGTCGTGGGTACCGGCTTTGTTCGGGGAACCGAAACCGATGATGGTTTTGCACATCAGCAGGGAAGGTTTGTCAGTCACTGCGCGCGCTTCTTCTACTGCGCGTTTGATAGATGCCGCGTCATGACCGTCGATGTCGCGAATAACGTGCCAGCCGTAAGCTTCGAAACGCATTGCGGTGTCGTCGGTGAACCA</t>
+          <t>CAATGACGTTACAGCTGCCGGTGTCTTTGCTGATCTGCTACGTACCCTCTCATGGAAGTTAGGAGTCTGACATGGTTAAAGTTTATGCCCCGGCTTCCAGTGCCAATATGAGCGTCGGGTTTGATGTGCTCGGGGCGGCGGTGACACCTGTTGATGGTGCATTGCTCGGAGATGTAGTCACGGTTGAGGCGGCAGAGACATTCAGTCTCAACAACCTCGGACGCTTTGCCGATAAGCTGCCGTCAGAACCACGGGAAAATATCGTTTATCAGTGCTGGGAGCGTTTTTGCCAGGAACTGGGTAAGCAAATTCCAGTGGCGATGACCCTGGAAAAGAATATGCCGATCGGTTCGGGCTTAGGCTCCAGTGCCTGTTCGGTGGTCGCGGCGCTGATGGCGATGAATGAACACTGCGGCAAGCCGCTTAATGACACTCGTTTGCTGGCTTTGATGGGCGAGCTGGAAGGCCGTATCTCCGGCAGCATTCATTACGACAACGTGGCACCGTGTTTTCTCGGTGGTATGCAGTTGATGATCGAAGAAAACGACATCATCAGCCAGCAAGTGCCAGGGTTTGATGAGTGGCTGTGGGTGCTGGCGTATCCGGGGATTAAAGTCTCGACGGCAGAAGCCAGGGCTATTTTACCGGCGCAGTATCGCCGCCAGGATTGCATTGCGCACGGGCGACATCTGGCAGGCTTCATTCACGCCTGCTATTCCCGTCAGCCTGAGCTTGCCGCGAAGCTGATGAAAGATGTTATCGCTGAACCCTACCGTGAACGGTTACTGCCAGGCTTCCGGCAGGCGCGGCAGGCGGTCGCGGAAATCGGCGCGGTAGCGAGCGGTATCTCCGGCTCCGGCCCGACCTTGTTCGCTCTGTGTGACAAGCCGGAAACCGCCCAGCGCGTTGCCGACTGGTTGGGTAAGAACTACCTGCAAAATCAGGAAGGTTTTGTTCATATTTGCCGGCTGGATACGGCGGGCGCACGAGTACTGGAAAACTAA</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>AGCAACAGCCAGTTCAACTTCTGAACCGGTAGCGATGAAAATCAGTTCCGGCTGACCGGCGCAGTCTTTCAGCACATAACCACCGCGCGCGATGTTTGCCAGTTGCTCTTCAGTTCGTTCCTGCTGCGCCAGGTTCTGACGGGAGAGGATCAGTGCGGTCGGGCCGTCCTGACGCTCAACACCGTATTTCCACGCGACCGCGGATTCAACCTGGTCACACGGACGCCATGTAGACATGTTCGGGGTTACGCGCAGAGAAGCGACCTGCTCAACCGGCTGGTGAGTCGGGCCGTCTTCGCCCAGACCGATGGAGTCGTGGGTGTAAACCATCACCTGACGCTGTTTCATCAGCGCAGCCATACGTACGGCGTTACGTGCGTATTCCACGAACATCAGGAAGGTGGAGGTGTACGGCAGGAAGCCACCGTGCAGGGAGATACCGTTAGCAATCGCGGTCATACCGAACTCGCGAACACCGTAGTGGATGTAGTTACCCGCAGCATCTTCGTTGATTGCTTTAGAACCAGACCACAGGGTCAGGTTAGACGGCGCCAGGTCAGCAGAACCGCCGAGGAATTCCGGCAACAGCGGACCGAACGCTTCGATAGCATTCTGAGACGCTTTACGGCTGGCGATTTTCGCCGGATTAGCCTGCAGTTTAGCGATGAACTCTTTCGCTTTAGCGTCGAAGTCAGACGGCATTTCGCCTTTCATACGGCGGGTAAATTCAGCGGCTTCCTGCGGATAAGCTTTCGCGTAAGCAGCGAATTTCTCGTTCCATGCGGATTCTTTCGCCTGGCCTGCTTCTTTCGCATCCCACTGAGCATAGATTTCAGACGGGATTTCGAACGGCGCATATTTCCAGCCCAGTTGTTCGCGGGTCAGGGCAATTTCAGCGTCGCCCAGCGGCGCACCGTGGGAGTCGTGGGTACCGGCTTTGTTCGGGGAACCGAAACCGATGATGGTTTTGCACATCAGCAGGGAAGGTTTGTCAGTCACTGCGCGCGCTTCTTCTACTGCGCGTTTGATAGATGCCGCGTCATGACCGTCGATGTCGCGAATAACGTGCCAGCCGTAAGCTTCGAAACGCATTGCGGTGTCGTCGGTGAACCA</t>
+          <t>GCCGCGTGAAGATTGCCGAAGTGGATGGTAATGATCCGCTGTTCAAAGTGAAAAATGGCGAAAACGCCCTGGCCTTCTATAGCCACTATTATCAGCCGCTGCCGTTGGTACTGCGCGGATATGGTGCGGGCAATGACGTTACAGCTGCCGGTGTCTTTGCTGATCTGCTACGTACCCTCTCATGGAAGTTAGGAGTCTGACATGGTTAAAGTTTATGCCCCGGCTTCCAGTGCCAATATGAGCGTCGGGTTTGATGTGCTCGGGGCGGCGGTGACACCTGTTGATGGTGCATTGCTCGGAGATGTAGTCACGGTTGAGGCGGCAGAGACATTCAGTCTCAACAACCTCGGACGCTTTGCCGATAAGCTGCCGTCAGAACCACGGGAAAATATCGTTTATCAGTGCTGGGAGCGTTTTTGCCAGGAACTGGGTAAGCAAATTCCAGTGGCGATGACCCTGGAAAAGAATATGCCGATCGGTTCGGGCTTAGGCTCCAGTGCCTGTTCGGTGGTCGCGGCGCTGATGGCGATGAATGAACACTGCGGCAAGCCGCTTAATGACACTCGTTTGCTGGCTTTGATGGGCGAGCTGGAAGGCCGTATCTCCGGCAGCATTCATTACGACAACGTGGCACCGTGTTTTCTCGGTGGTATGCAGTTGATGATCGAAGAAAACGACATCATCAGCCAGCAAGTGCCAGGGTTTGATGAGTGGCTGTGGGTGCTGGCGTATCCGGGGATTAAAGTCTCGACGGCAGAAGCCAGGGCTATTTTACCGGCGCAGTATCGCCGCCAGGATTGCATTGCGCACGGGCGACATCTGGCAGGCTTCATTCACGCCTGCTATTCCCGTCAGCCTGAGCTTGCCGCGAAGCTGATGAAAGATGTTATCGCTGAACCCTACCGTGAACGGTTACTGCCAGGCTTCCGGCAGGCGCGGCAGGCGGTCGCGGAAATCGGCGCGGTAGCGAGCGGTATCTCCGGCTCCGGCCCGACCTTGTTCGCTCTGTGTGACAAGCCGGAAACCGCCCAGCGCGTTGCCGACTGGTTGGGTAAGAACTACCTGCAAAATCAGGAAGGTTTTGTTCATATTTGCCGGCTGGATACGGCGGGCGCACGAGTACTGGAAAACTAA</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>AGGTTCTGACGGGAGAGGATCAGTGCGGTCGGGCCGTCCTGACGCTCAACACCGTATTTCCACGCGACCGCGGATTCAACCTGGTCACACGGACGCCATGTAGACATGTTCGGGGTTACGCGCAGAGAAGCGACCTGCTCAACCGGCTGGTGAGTCGGGCCGTCTTCGCCCAGACCGATGGAGTCGTGGGTGTAAACCATCACCTGACGCTGTTTCATCAGCGCAGCCATACGTACGGCGTTACGTGCGTATTCCACGAACATCAGGAAGGTGGAGGTGTACGGCAGGAAGCCACCGTGCAGGGAGATACCGTTAGCAATCGCGGTCATACCGAACTCGCGAACACCGTAGTGGATGTAGTTACCCGCAGCATCTTCGTTGATTGCTTTAGAACCAGACCACAGGGTCAGGTTAGACGGCGCCAGGTCAGCAGAACCGCCGAGGAATTCCGGCAACAGCGGACCGAACGCTTCGATAGCATTCTGAGACGCTTTACGGCTGGCGATTTTCGCCGGATTAGCCTGCAGTTTAGCGATGAACTCTTTCGCTTTAGCGTCGAAGTCAGACGGCATTTCGCCTTTCATACGGCGGGTAAATTCAGCGGCTTCCTGCGGATAAGCTTTCGCGTAAGCAGCGAATTTCTCGTTCCATGCGGATTCTTTCGCCTGGCCTGCTTCTTTCGCATCCCACTGAGCATAGATTTCAGACGGGATTTCGAACGGCGCATATTTCCAGCCCAGTTGTTCGCGGGTCAGGGCAATTTCAGCGTCGCCCAGCGGCGCACCGTGGGAGTCGTGGGTACCGGCTTTGTTCGGGGAACCGAAACCGATGATGGTTTTGCACATCAGCAGGGAAGGTTTGTCAGTCACTGCGCGCGCTTCTTCTACTGCGCGTTTGATAGATGCCGCGTCATGACCGTCGATGTCGCGAATAACGTGCCAGCCGTAAGCTTCGAAACGCATTGCGGTGTCGTCGGTGAACCATCCCTCGACATGAATAGGCGTATCACGAGGCC</t>
+          <t>CAATGACGTTACAGCTGCCGGTGTCTTTGCTGATCTGCTACGTACCCTCTCATGGAAGTTAGGAGTCTGACATGGTTAAAGTTTATGCCCCGGCTTCCAGTGCCAATATGAGCGTCGGGTTTGATGTGCTCGGGGCGGCGGTGACACCTGTTGATGGTGCATTGCTCGGAGATGTAGTCACGGTTGAGGCGGCAGAGACATTCAGTCTCAACAACCTCGGACGCTTTGCCGATAAGCTGCCGTCAGAACCACGGGAAAATATCGTTTATCAGTGCTGGGAGCGTTTTTGCCAGGAACTGGGTAAGCAAATTCCAGTGGCGATGACCCTGGAAAAGAATATGCCGATCGGTTCGGGCTTAGGCTCCAGTGCCTGTTCGGTGGTCGCGGCGCTGATGGCGATGAATGAACACTGCGGCAAGCCGCTTAATGACACTCGTTTGCTGGCTTTGATGGGCGAGCTGGAAGGCCGTATCTCCGGCAGCATTCATTACGACAACGTGGCACCGTGTTTTCTCGGTGGTATGCAGTTGATGATCGAAGAAAACGACATCATCAGCCAGCAAGTGCCAGGGTTTGATGAGTGGCTGTGGGTGCTGGCGTATCCGGGGATTAAAGTCTCGACGGCAGAAGCCAGGGCTATTTTACCGGCGCAGTATCGCCGCCAGGATTGCATTGCGCACGGGCGACATCTGGCAGGCTTCATTCACGCCTGCTATTCCCGTCAGCCTGAGCTTGCCGCGAAGCTGATGAAAGATGTTATCGCTGAACCCTACCGTGAACGGTTACTGCCAGGCTTCCGGCAGGCGCGGCAGGCGGTCGCGGAAATCGGCGCGGTAGCGAGCGGTATCTCCGGCTCCGGCCCGACCTTGTTCGCTCTGTGTGACAAGCCGGAAACCGCCCAGCGCGTTGCCGACTGGTTGGGTAAGAACTACCTGCAAAATCAGGAAGGTTTTGTTCATATTTGCCGGCTGGATACGGCGGGCGCACGAGTACTGGAAAACTAAAATAGGCGTATCACGAGGCC</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>1015</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="4">
@@ -556,112 +556,36 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>aceE_del</t>
+          <t>b0005</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>GCGTCACAGACATGAAATTGGT</t>
+          <t>TCTGTACATTGGGCGGCAAT</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>GGCCTCGTGATACGCCTATTGGGTTATTCCTTATCTATCT</t>
+          <t>GGCCTCGTGATACGCCTATTAGGTTACTCCTTTTATCATTGCCC</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>GCGTCACAGACATGAAATTGGTAAGACCAATTGACTTCGGCAAGTGGCTTAAGACAGGAACTCATGGCCTACAGCAAAATCCGCCAACCAAAACTCTCCGATGTGATTGAGCAGCAACTGGAGTTTTTGATCCTCGAAGGCACTCTCCGCCCGGGCGAAAAACTCCCACCGGAACGCGAACTGGCAAAACAGTTTGACGTCTCCCGTCCCTCCTTGCGTGAGGCGATTCAACGTCTCGAAGCGAAGGGCTTGTTGCTTCGTCGCCAGGGTGGCGGCACTTTTGTCCAGAGCAGCCTATGGCAAAGCTTCAGCGATCCGCTGGTGGAGCTGCTCTCCGACCATCCTGAGTCACAGTATGACTTGCTCGAAACACGACACGCCCTGGAAGGTATCGCCGCTTATTACGCCGCGCTGCGTAGTACCGATGAAGACAAGGAACGCATCCGTGAACTCCACCACGCCATAGAGCTGGCGCAGCAGTCTGGCGATCTGGACGCGGAATCAAACGCCGTACTCCAGTATCAGATTGCCGTCACCGAAGCGGCCCACAATGTGGTTCTGCTTCATCTGCTAAGGTGTATGGAGCCGATGTTGGCCCAGAATGTCCGCCAGAACTTCGAATTGCTCTATTCGCGTCGCGAGATGCTGCCGCTGGTGAGTAGTCACCGCACCCGCATATTTGAAGCGATTATGGCCGGTAAGCCGGAAGAAGCGCGCGAAGCATCGCATCGCCATCTGGCCTTTATCGAAGAAATTTTGCTCGACAGAAGTCGTGAAGAGAGCCGCCGTGAGCGTTCTCTGCGTCGTCTGGAGCAACGAAAGAATTAGTGATTTTTCTGGTAAAAATTATCCAGAAGATGTTGTAAATCAAGCGCATATAAAAGCGCGGCAACTAAACGTAGAACCTGTCTTATTGAGCTTTCCGGCGAGAGTTCAATGGGACAGGTTCCAGAAAACTCAACGTTATTAGATAGATAAGGAATAACCC</t>
+          <t>TCTGTACATTGGGCGGCAATATCGAAACTGTTGCCATCGACGGCGATTTCGATGCCTGTCAGGCGCTGGTGAAGCAGGCGTTTGATGATGAAGAACTGAAAGTGGCGCTAGGGTTAAACTCGGCTAACTCGATTAACATCAGCCGTTTGCTGGCGCAGATTTGCTACTACTTTGAAGCTGTTGCGCAGCTGCCGCAGGAGACGCGCAACCAGCTGGTTGTCTCGGTGCCAAGCGGAAACTTCGGCGATTTGACGGCGGGTCTGCTGGCGAAGTCACTCGGTCTGCCGGTGAAACGTTTTATTGCTGCGACCAACGTGAACGATACCGTGCCACGTTTCCTGCACGACGGTCAGTGGTCACCCAAAGCGACTCAGGCGACGTTATCCAACGCGATGGACGTGAGTCAGCCGAACAACTGGCCGCGTGTGGAAGAGTTGTTCCGCCGCAAAATCTGGCAACTGAAAGAGCTGGGTTATGCAGCCGTGGATGATGAAACCACGCAACAGACAATGCGTGAGTTAAAAGAACTGGGCTACACTTCGGAGCCGCACGCTGCCGTAGCTTATCGTGCGCTGCGTGATCAGTTGAATCCAGGCGAATATGGCTTGTTCCTCGGCACCGCGCATCCGGCGAAATTTAAAGAGAGCGTGGAAGCGATTCTCGGTGAAACGTTGGATCTGCCAAAAGAGCTGGCAGAACGTGCTGATTTACCCTTGCTTTCACATAATCTGCCCGCCGATTTTGCTGCGTTGCGTAAATTGATGATGAATCATCAGTAAAATCTATTCATTATCTCAATCAGGCCGGGTTTGCTTTTATGCAGCCCGGCTTTTTTATGAAGAAATTATGGAGAAAAATGACAGGGAAAAAGGAGAAATTCTCAATAAATGCGGTAACTTAGAGATTAGGATTGCGGAGAATAACAACCGCCGTTCTCATCGAGTAATCTCCGGATATCGACCCATAACGGGCAATGATAAAAGGAGTAACCT</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>TACGTAAAGTCTACATTTGTGCATAGTTACAACTTTGAAACGTTATATATGTCAAGTTGTTAAAATGTGCACAGTTTCATGATTTCAATCAAAACCTGTATGGACATAAGGTGAATACTTTGTTACTTTAGCGTCACAGACATGAAATTGGTAAGACCAATTGACTTCGGCAAGTGGCTTAAGACAGGAACTCATGGCCTACAGCAAAATCCGCCAACCAAAACTCTCCGATGTGATTGAGCAGCAACTGGAGTTTTTGATCCTCGAAGGCACTCTCCGCCCGGGCGAAAAACTCCCACCGGAACGCGAACTGGCAAAACAGTTTGACGTCTCCCGTCCCTCCTTGCGTGAGGCGATTCAACGTCTCGAAGCGAAGGGCTTGTTGCTTCGTCGCCAGGGTGGCGGCACTTTTGTCCAGAGCAGCCTATGGCAAAGCTTCAGCGATCCGCTGGTGGAGCTGCTCTCCGACCATCCTGAGTCACAGTATGACTTGCTCGAAACACGACACGCCCTGGAAGGTATCGCCGCTTATTACGCCGCGCTGCGTAGTACCGATGAAGACAAGGAACGCATCCGTGAACTCCACCACGCCATAGAGCTGGCGCAGCAGTCTGGCGATCTGGACGCGGAATCAAACGCCGTACTCCAGTATCAGATTGCCGTCACCGAAGCGGCCCACAATGTGGTTCTGCTTCATCTGCTAAGGTGTATGGAGCCGATGTTGGCCCAGAATGTCCGCCAGAACTTCGAATTGCTCTATTCGCGTCGCGAGATGCTGCCGCTGGTGAGTAGTCACCGCACCCGCATATTTGAAGCGATTATGGCCGGTAAGCCGGAAGAAGCGCGCGAAGCATCGCATCGCCATCTGGCCTTTATCGAAGAAATTTTGCTCGACAGAAGTCGTGAAGAGAGCCGCCGTGAGCGTTCTCTGCGTCGTCTGGAGCAACGAAAGAATTAGTGATTTTTCTGGTAAAAATTATCCAGAAGATGTTGTAAATCAAGCGCATATAAAAGCGCGGCAACTAAACGTAGAACCTGTCTTATTGAGCTTTCCGGCGAGAGTTCAATGGGACAGGTTCCAGAAAACTCAACGTTATTAGATAGATAAGGAATAACCC</t>
+          <t>GTGACCATTCTGACCGCGACCTCCGGTGATACCGGAGCGGCAGTGGCTCATGCTTTCTACGGTTTACCGAATGTGAAAGTGGTTATCCTCTATCCACGAGGCAAAATCAGTCCACTGCAAGAAAAACTGTTCTGTACATTGGGCGGCAATATCGAAACTGTTGCCATCGACGGCGATTTCGATGCCTGTCAGGCGCTGGTGAAGCAGGCGTTTGATGATGAAGAACTGAAAGTGGCGCTAGGGTTAAACTCGGCTAACTCGATTAACATCAGCCGTTTGCTGGCGCAGATTTGCTACTACTTTGAAGCTGTTGCGCAGCTGCCGCAGGAGACGCGCAACCAGCTGGTTGTCTCGGTGCCAAGCGGAAACTTCGGCGATTTGACGGCGGGTCTGCTGGCGAAGTCACTCGGTCTGCCGGTGAAACGTTTTATTGCTGCGACCAACGTGAACGATACCGTGCCACGTTTCCTGCACGACGGTCAGTGGTCACCCAAAGCGACTCAGGCGACGTTATCCAACGCGATGGACGTGAGTCAGCCGAACAACTGGCCGCGTGTGGAAGAGTTGTTCCGCCGCAAAATCTGGCAACTGAAAGAGCTGGGTTATGCAGCCGTGGATGATGAAACCACGCAACAGACAATGCGTGAGTTAAAAGAACTGGGCTACACTTCGGAGCCGCACGCTGCCGTAGCTTATCGTGCGCTGCGTGATCAGTTGAATCCAGGCGAATATGGCTTGTTCCTCGGCACCGCGCATCCGGCGAAATTTAAAGAGAGCGTGGAAGCGATTCTCGGTGAAACGTTGGATCTGCCAAAAGAGCTGGCAGAACGTGCTGATTTACCCTTGCTTTCACATAATCTGCCCGCCGATTTTGCTGCGTTGCGTAAATTGATGATGAATCATCAGTAAAATCTATTCATTATCTCAATCAGGCCGGGTTTGCTTTTATGCAGCCCGGCTTTTTTATGAAGAAATTATGGAGAAAAATGACAGGGAAAAAGGAGAAATTCTCAATAAATGCGGTAACTTAGAGATTAGGATTGCGGAGAATAACAACCGCCGTTCTCATCGAGTAATCTCCGGATATCGACCCATAACGGGCAATGATAAAAGGAGTAACCT</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>GCGTCACAGACATGAAATTGGTAAGACCAATTGACTTCGGCAAGTGGCTTAAGACAGGAACTCATGGCCTACAGCAAAATCCGCCAACCAAAACTCTCCGATGTGATTGAGCAGCAACTGGAGTTTTTGATCCTCGAAGGCACTCTCCGCCCGGGCGAAAAACTCCCACCGGAACGCGAACTGGCAAAACAGTTTGACGTCTCCCGTCCCTCCTTGCGTGAGGCGATTCAACGTCTCGAAGCGAAGGGCTTGTTGCTTCGTCGCCAGGGTGGCGGCACTTTTGTCCAGAGCAGCCTATGGCAAAGCTTCAGCGATCCGCTGGTGGAGCTGCTCTCCGACCATCCTGAGTCACAGTATGACTTGCTCGAAACACGACACGCCCTGGAAGGTATCGCCGCTTATTACGCCGCGCTGCGTAGTACCGATGAAGACAAGGAACGCATCCGTGAACTCCACCACGCCATAGAGCTGGCGCAGCAGTCTGGCGATCTGGACGCGGAATCAAACGCCGTACTCCAGTATCAGATTGCCGTCACCGAAGCGGCCCACAATGTGGTTCTGCTTCATCTGCTAAGGTGTATGGAGCCGATGTTGGCCCAGAATGTCCGCCAGAACTTCGAATTGCTCTATTCGCGTCGCGAGATGCTGCCGCTGGTGAGTAGTCACCGCACCCGCATATTTGAAGCGATTATGGCCGGTAAGCCGGAAGAAGCGCGCGAAGCATCGCATCGCCATCTGGCCTTTATCGAAGAAATTTTGCTCGACAGAAGTCGTGAAGAGAGCCGCCGTGAGCGTTCTCTGCGTCGTCTGGAGCAACGAAAGAATTAGTGATTTTTCTGGTAAAAATTATCCAGAAGATGTTGTAAATCAAGCGCATATAAAAGCGCGGCAACTAAACGTAGAACCTGTCTTATTGAGCTTTCCGGCGAGAGTTCAATGGGACAGGTTCCAGAAAACTCAACGTTATTAGATAGATAAGGAATAACCCAATAGGCGTATCACGAGGCC</t>
+          <t>TCTGTACATTGGGCGGCAATATCGAAACTGTTGCCATCGACGGCGATTTCGATGCCTGTCAGGCGCTGGTGAAGCAGGCGTTTGATGATGAAGAACTGAAAGTGGCGCTAGGGTTAAACTCGGCTAACTCGATTAACATCAGCCGTTTGCTGGCGCAGATTTGCTACTACTTTGAAGCTGTTGCGCAGCTGCCGCAGGAGACGCGCAACCAGCTGGTTGTCTCGGTGCCAAGCGGAAACTTCGGCGATTTGACGGCGGGTCTGCTGGCGAAGTCACTCGGTCTGCCGGTGAAACGTTTTATTGCTGCGACCAACGTGAACGATACCGTGCCACGTTTCCTGCACGACGGTCAGTGGTCACCCAAAGCGACTCAGGCGACGTTATCCAACGCGATGGACGTGAGTCAGCCGAACAACTGGCCGCGTGTGGAAGAGTTGTTCCGCCGCAAAATCTGGCAACTGAAAGAGCTGGGTTATGCAGCCGTGGATGATGAAACCACGCAACAGACAATGCGTGAGTTAAAAGAACTGGGCTACACTTCGGAGCCGCACGCTGCCGTAGCTTATCGTGCGCTGCGTGATCAGTTGAATCCAGGCGAATATGGCTTGTTCCTCGGCACCGCGCATCCGGCGAAATTTAAAGAGAGCGTGGAAGCGATTCTCGGTGAAACGTTGGATCTGCCAAAAGAGCTGGCAGAACGTGCTGATTTACCCTTGCTTTCACATAATCTGCCCGCCGATTTTGCTGCGTTGCGTAAATTGATGATGAATCATCAGTAAAATCTATTCATTATCTCAATCAGGCCGGGTTTGCTTTTATGCAGCCCGGCTTTTTTATGAAGAAATTATGGAGAAAAATGACAGGGAAAAAGGAGAAATTCTCAATAAATGCGGTAACTTAGAGATTAGGATTGCGGAGAATAACAACCGCCGTTCTCATCGAGTAATCTCCGGATATCGACCCATAACGGGCAATGATAAAAGGAGTAACCTAATAGGCGTATCACGAGGCC</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>pntA_promoter_sub</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CGAGGTTTGTGCCGTAAAGC</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>GGCCTCGTGATACGCCTATTGTCCTAGGTATAATGCTAGCACGAATCTAGAGAAAGATTGGACGTACCATAATGCGAATTGGCATACCAAGAG</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>CGAGGTTTGTGCCGTAAAGCTGTGAGGATTGCGTCGGCAGACGGCCCGGAAGATCGGTATAACCAATCACTTTGACACCATTTTCCGTAGTGAAGATTTCACCCGGCACGGTGTATTCACAGTTGCCGCCGTTTTGGGCTGCCAGGTCGACAATCACACTGCCCGCCTTCATGGAGTCAACCATTTCACGGGTAATTAGCTTCGGCGCTGGTTTGCCTGGAATAAGCGCGGTGGTGACAATGATATCGACCTCTTTTGCCTGGGCGGCAAAGAGTTCCATTTCCGCTTTGATGAACGCGTCCGACATCACTTTGGCATAGCCATCGCCGCTGCCAGCTTCCTCTTTAAAATCCAGCTCGAGGAATTCCGCGCCCATACTTTGAACTTGTTCTTTCACTTCCGGGCGGGTGTCGAATGCACGCACAATCGCGCCGAGACTGTTTGCTGCGCCAATGGCGGCCAGACCTGCAACACCCGCACCAATCACCATCACTTTTGCCGGTGGCACTTTCCCGGCCGCAGTAATTTGCCCGGTAAAGAAGCGCCCAAATTCATGTGCCGCTTCAACAATGGCGCGATAACCGGCGATGTTCGCCATCGAGCTTAGTGCGTCCAGCGATTGTGCGCGTGAGATACGCGGCACAGAGTCCATCGCCATCACGGTCACGTTACGTTCCGCAAGTTTTTGCATTAATTCCGGATTCTGCGCAGGCCAGATAAAACTCACCAGCGTTGTCCCAGGATTCAGTAACGCAATTTCATCATCTAACGGCGCATTGACCTTCAGAATGATCTCTGACTGCCAGACGCTATTCCCTTCTACAATTTCAGCGCCCGCTTGCACAAACGCTTTATCGTCAAAACTTGCCAGTTGACCCGCGCCGCTCTCTACCGCGACGGTAAAACCCAGTTTCAGCAGCTGTTCCACTGTTTTTGGCGTTGCTGCAACACGGGTTTCATTGGTTAACCGTTCTCTTGGTATGCCAATTCGCAT</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>ACCTGAATCGGCGGTGCCGGCCAGGTAATTTCGCCCGCACGGATCACGGTCACGCCGCGAATCACCACATCATCAAAATCAACAGTGATATTGCCGTCTTTCTCTTTGCACAACAGTTTCAGCAGATTAACGAGGTTTGTGCCGTAAAGCTGTGAGGATTGCGTCGGCAGACGGCCCGGAAGATCGGTATAACCAATCACTTTGACACCATTTTCCGTAGTGAAGATTTCACCCGGCACGGTGTATTCACAGTTGCCGCCGTTTTGGGCTGCCAGGTCGACAATCACACTGCCCGCCTTCATGGAGTCAACCATTTCACGGGTAATTAGCTTCGGCGCTGGTTTGCCTGGAATAAGCGCGGTGGTGACAATGATATCGACCTCTTTTGCCTGGGCGGCAAAGAGTTCCATTTCCGCTTTGATGAACGCGTCCGACATCACTTTGGCATAGCCATCGCCGCTGCCAGCTTCCTCTTTAAAATCCAGCTCGAGGAATTCCGCGCCCATACTTTGAACTTGTTCTTTCACTTCCGGGCGGGTGTCGAATGCACGCACAATCGCGCCGAGACTGTTTGCTGCGCCAATGGCGGCCAGACCTGCAACACCCGCACCAATCACCATCACTTTTGCCGGTGGCACTTTCCCGGCCGCAGTAATTTGCCCGGTAAAGAAGCGCCCAAATTCATGTGCCGCTTCAACAATGGCGCGATAACCGGCGATGTTCGCCATCGAGCTTAGTGCGTCCAGCGATTGTGCGCGTGAGATACGCGGCACAGAGTCCATCGCCATCACGGTCACGTTACGTTCCGCAAGTTTTTGCATTAATTCCGGATTCTGCGCAGGCCAGATAAAACTCACCAGCGTTGTCCCAGGATTCAGTAACGCAATTTCATCATCTAACGGCGCATTGACCTTCAGAATGATCTCTGACTGCCAGACGCTATTCCCTTCTACAATTTCAGCGCCCGCTTGCACAAACGCTTTATCGTCAAAACTTGCCAGTTGACCCGCGCCGCTCTCTACCGCGACGGTAAAACCCAGTTTCAGCAGCTGTTCCACTGTTTTTGGCGTTGCTGCAACACGGGTTTCATTGGTTAACCGTTCTCTTGGTATGCCAATTCGCAT</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>CGAGGTTTGTGCCGTAAAGCTGTGAGGATTGCGTCGGCAGACGGCCCGGAAGATCGGTATAACCAATCACTTTGACACCATTTTCCGTAGTGAAGATTTCACCCGGCACGGTGTATTCACAGTTGCCGCCGTTTTGGGCTGCCAGGTCGACAATCACACTGCCCGCCTTCATGGAGTCAACCATTTCACGGGTAATTAGCTTCGGCGCTGGTTTGCCTGGAATAAGCGCGGTGGTGACAATGATATCGACCTCTTTTGCCTGGGCGGCAAAGAGTTCCATTTCCGCTTTGATGAACGCGTCCGACATCACTTTGGCATAGCCATCGCCGCTGCCAGCTTCCTCTTTAAAATCCAGCTCGAGGAATTCCGCGCCCATACTTTGAACTTGTTCTTTCACTTCCGGGCGGGTGTCGAATGCACGCACAATCGCGCCGAGACTGTTTGCTGCGCCAATGGCGGCCAGACCTGCAACACCCGCACCAATCACCATCACTTTTGCCGGTGGCACTTTCCCGGCCGCAGTAATTTGCCCGGTAAAGAAGCGCCCAAATTCATGTGCCGCTTCAACAATGGCGCGATAACCGGCGATGTTCGCCATCGAGCTTAGTGCGTCCAGCGATTGTGCGCGTGAGATACGCGGCACAGAGTCCATCGCCATCACGGTCACGTTACGTTCCGCAAGTTTTTGCATTAATTCCGGATTCTGCGCAGGCCAGATAAAACTCACCAGCGTTGTCCCAGGATTCAGTAACGCAATTTCATCATCTAACGGCGCATTGACCTTCAGAATGATCTCTGACTGCCAGACGCTATTCCCTTCTACAATTTCAGCGCCCGCTTGCACAAACGCTTTATCGTCAAAACTTGCCAGTTGACCCGCGCCGCTCTCTACCGCGACGGTAAAACCCAGTTTCAGCAGCTGTTCCACTGTTTTTGGCGTTGCTGCAACACGGGTTTCATTGGTTAACCGTTCTCTTGGTATGCCAATTCGCATTATGGTACGTCCAATCTTTCTCTAGATTCGTGCTAGCATTATACCTAGGACAATAGGCGTATCACGAGGCC</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Cgl1452_ins</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CACTGCGCGGGATTTTATGG</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>TCAATACTCTTTTTGGCGCGCATGTGAACGCCTGACCAGG</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>CACTGCGCGGGATTTTATGGAGATTCACTTACCTAAAGATTTACGTGAACTGTGCGATCTCGATAGCTTAAAACTGGAATCCGCCAGCTTTGTCGATGAAAAATTGCGGGCGCTACACTCCGATATTTTATGGTCGGTAAAGACCCGCGAAGGCGATGGCTATATCTATGTGGTGATTGAACATCAGAGCCGCGAGGACATTCATATGGCCTTTCGCCTGATGCGCTATTCCATGGCGGTGATGTAGCGCCATATAGAGCATGATAAACGCCAGCCGCTACCGTTGGTCATCCCGATGCTATTTTATCACGGTAGCCGTAGTCCTTACCCCTGGTCCCTGTGCTGGCTGGACGAATTTGCCGACCCGACTACCGCACGGAAGCTTTATAACGCCGCGTTCCCGCTGGTGGATGTTACTGTCGTGCCAGACGACGAGATTGTGCAGCATCGCAGAGTCGCCCTGTTGGAGTTGATCCAAAAGCATATTCGCCAGCGCGATCTGATGGGGCTTATCGATCAACTGGTAGTATTACTGGTTACAGAGTGTGCTAATGACAGCCAGATAACTGCGCTGTTAAATTACATTTTACTGACTGGCGATGAAGCGCGTTTTAATGAGTTTATCAGTGAACTTACCCGTCGAATGCCACAACACAGGGAGCGAATAATGACGATTGCAGAGCGAATTCATAATGATGGATATATAAAAGGGGAGCAGCGCATTCTTCGATTGTTGTTGCAGAATGGGGCGGATCCTGAATGGATACAAAAGATTACCGGACTTTCGGCAGAGCAAATGCAGGCATTAAGGCAGCCCTTGCCTGAGCGTGAGCGCTATTCATGGCTCAAGAGCTAATCAGAGACGGATGACAAACGCAAAGCAGCCTGATGCGCTATGCTTATCAGGTCTACATAACCCATTAAATATATTGAACTTTAAAGATTTTTGTAGACCTGGTCAGGCGTTCACATG</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>CGGGTGAGAATGGTTTTGTTAGTCGCTAAAGTCAGGCCATCTTTTTCAACAGGTGATGGATCGCCATGACAAACTTCACGACCAGCACGCCGCATGATGCATTATTTAAAACCTTTCTCACGCACCCTGACACTGCGCGGGATTTTATGGAGATTCACTTACCTAAAGATTTACGTGAACTGTGCGATCTCGATAGCTTAAAACTGGAATCCGCCAGCTTTGTCGATGAAAAATTGCGGGCGCTACACTCCGATATTTTATGGTCGGTAAAGACCCGCGAAGGCGATGGCTATATCTATGTGGTGATTGAACATCAGAGCCGCGAGGACATTCATATGGCCTTTCGCCTGATGCGCTATTCCATGGCGGTGATGTAGCGCCATATAGAGCATGATAAACGCCAGCCGCTACCGTTGGTCATCCCGATGCTATTTTATCACGGTAGCCGTAGTCCTTACCCCTGGTCCCTGTGCTGGCTGGACGAATTTGCCGACCCGACTACCGCACGGAAGCTTTATAACGCCGCGTTCCCGCTGGTGGATGTTACTGTCGTGCCAGACGACGAGATTGTGCAGCATCGCAGAGTCGCCCTGTTGGAGTTGATCCAAAAGCATATTCGCCAGCGCGATCTGATGGGGCTTATCGATCAACTGGTAGTATTACTGGTTACAGAGTGTGCTAATGACAGCCAGATAACTGCGCTGTTAAATTACATTTTACTGACTGGCGATGAAGCGCGTTTTAATGAGTTTATCAGTGAACTTACCCGTCGAATGCCACAACACAGGGAGCGAATAATGACGATTGCAGAGCGAATTCATAATGATGGATATATAAAAGGGGAGCAGCGCATTCTTCGATTGTTGTTGCAGAATGGGGCGGATCCTGAATGGATACAAAAGATTACCGGACTTTCGGCAGAGCAAATGCAGGCATTAAGGCAGCCCTTGCCTGAGCGTGAGCGCTATTCATGGCTCAAGAGCTAATCAGAGACGGATGACAAACGCAAAGCAGCCTGATGCGCTATGCTTATCAGGTCTACATAACCCATTAAATATATTGAACTTTAAAGATTTTTGTAGACCTGGTCAGGCGTTCACATG</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>CACTGCGCGGGATTTTATGGAGATTCACTTACCTAAAGATTTACGTGAACTGTGCGATCTCGATAGCTTAAAACTGGAATCCGCCAGCTTTGTCGATGAAAAATTGCGGGCGCTACACTCCGATATTTTATGGTCGGTAAAGACCCGCGAAGGCGATGGCTATATCTATGTGGTGATTGAACATCAGAGCCGCGAGGACATTCATATGGCCTTTCGCCTGATGCGCTATTCCATGGCGGTGATGTAGCGCCATATAGAGCATGATAAACGCCAGCCGCTACCGTTGGTCATCCCGATGCTATTTTATCACGGTAGCCGTAGTCCTTACCCCTGGTCCCTGTGCTGGCTGGACGAATTTGCCGACCCGACTACCGCACGGAAGCTTTATAACGCCGCGTTCCCGCTGGTGGATGTTACTGTCGTGCCAGACGACGAGATTGTGCAGCATCGCAGAGTCGCCCTGTTGGAGTTGATCCAAAAGCATATTCGCCAGCGCGATCTGATGGGGCTTATCGATCAACTGGTAGTATTACTGGTTACAGAGTGTGCTAATGACAGCCAGATAACTGCGCTGTTAAATTACATTTTACTGACTGGCGATGAAGCGCGTTTTAATGAGTTTATCAGTGAACTTACCCGTCGAATGCCACAACACAGGGAGCGAATAATGACGATTGCAGAGCGAATTCATAATGATGGATATATAAAAGGGGAGCAGCGCATTCTTCGATTGTTGTTGCAGAATGGGGCGGATCCTGAATGGATACAAAAGATTACCGGACTTTCGGCAGAGCAAATGCAGGCATTAAGGCAGCCCTTGCCTGAGCGTGAGCGCTATTCATGGCTCAAGAGCTAATCAGAGACGGATGACAAACGCAAAGCAGCCTGATGCGCTATGCTTATCAGGTCTACATAACCCATTAAATATATTGAACTTTAAAGATTTTTGTAGACCTGGTCAGGCGTTCACATGCGCGCCAAAAAGAGTATTGA</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>993</v>
+        <v>1012</v>
       </c>
     </row>
   </sheetData>
@@ -675,7 +599,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -726,35 +650,35 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dxs_sub_933_C_T_sub</t>
+          <t>b0003</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CAGTCACTCGATACCTCGGC</t>
+          <t>GCATTGTCTGTTGCGTGGTT</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CAAATAAAACGAAAGGCTCATAGCTCGGCAAACCGCCGCTACTTTTCGGTAAACAACCGCTGGAGGGATC</t>
+          <t>CAAATAAAACGAAAGGCTCAGTACCCTCTCATGGAAGTTAGGAGTCTGACATGAAACTCTACAATCTGAAAGA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CAAATAAAACGAAAGGCTCATAGCTCGGCAAACCGCCGCTACTTTTCGGTAAACAACCGCTGGAGGGATCAAATTTAGGCACGGCGTGGAAAGTGATCGGGTCTTTTTCTGCCGGTTCATAACCACGACCTTTTTTGGTCATGATATGCAGGAACTGCGGGCCTTTCAGGTCGCGCATGTTCTTTAGCGTGGTGATAAGCCCCAGCACATCGTGACCGTCCACCGGGCCGATGTAGTTAAAGCCCAGCTCTTCAAACAACGTGCCAGGCACTACCATGCCTTTAATATGTTCTTCGGTGCGTTTGAGCAGCTCTTTAATTGGCGGCACGCCAGAGAAAACTTTTTTCCCGCCTTCGCGCAGTGAAGAGTAAAGCTTACCGGAAAGCAGCTGTGCCAGATGGTTGTTGAGCGCGCCGACATTTTCGGAAATCGACATTTCATTGTCGTTGAGAATCACCAGCATATCAGGACGGATATCGCCCGCGTGATTCATCGCTTCAAACGCCATGCCTGCGGTAATCGCGCCATCGCCAATGACACAGACGGTGCGGCGATTTTTGCCTTCTTTTTCGGCAGCAACCGCAATACCAATTCCGGCACTGATGGAGGTTGATGAATGCCCGACGCTTAATACGTCATATTCGCTTTCGCCGCGCCACGGGAACGGGTGCAGACCGCCTTTCTGACGGATGGTGCCGATTTTGTCGCGGCGTCCGGTCAAAATTTTATGCGGATAAGCCTGATGCCCCACATCCCAAATCAATTGGTCAAACGGGGTGTTGTAGACATAGTGCAGCGCCACGGTCAGTTCGACCGTGCCCAGCCCGGAGGCGAAGTGCCCGCTGGAACGGCTCACGCTGTCGAGTAAATAGCGGCGCAGTTCGTCGCAGAGTTTCGGTAAACTCTCTTTCGGCAACAGTCGTAACTCCTGGGTGGAGTCGACCAGTGCCAGGGTCGGGTATTTGGCAATATCAAAACTCATCAGGGGCCTATTAATACTTATTGTTTATTTATTACGCTGGATGATGTAGTCCGCTAGCGCTTCCAGTGCCGAGGTATCGAGTGACTG</t>
+          <t>CAAATAAAACGAAAGGCTCAGTACCCTCTCATGGAAGTTAGGAGTCTGACATGAAACTCTACAATCTGAAAGATCACAACGAGCAGGTCAGCTTTGCGCAAGCCGTAACCCAGGGGTTGGGCAAAAATCAGGGGCTGTTTTTTCCGCACGACCTGCCGGAATTCAGCCTGACTGAAATTGATGAGATGCTGAAGCTGGATTTTGTCACCCGCAGTGCGAAGATCCTCTCGGCGTTTATTGGTGATGAAATCCCACAGGAAATCCTGGAAGAGCGCGTGCGCGCGGCGTTTGCCTTCCCGGCTCCGGTCGCCAATGTTGAAAGCGATGTCGGTTGTCTGGAATTGTTCCACGGGCCAACGCTGGCATTTAAAGATTTCGGCGGTCGCTTTATGGCACAAATGCTGACCCATATTGCGGGTGATAAGCCAGTGACCATTCTGACCGCGACCTCCGGTGATACCGGAGCGGCAGTGGCTCATGCTTTCTACGGTTTACCGAATGTGAAAGTGGTTATCCTCTATCCACGAGGCAAAATCAGTCCACTGCAAGAAAAACTGTTCTGTACATTGGGCGGCAATATCGAAACTGTTGCCATCGACGGCGATTTCGATGCCTGTCAGGCGCTGGTGAAGCAGGCGTTTGATGATGAAGAACTGAAAGTGGCGCTAGGGTTAAACTCGGCTAACTCGATTAACATCAGCCGTTTGCTGGCGCAGATTTGCTACTACTTTGAAGCTGTTGCGCAGCTGCCGCAGGAGACGCGCAACCAGCTGGTTGTCTCGGTGCCAAGCGGAAACTTCGGCGATTTGACGGCGGGTCTGCTGGCGAAGTCACTCGGTCTGCCGGTGAAACGTTTTATTGCTGCGACCAACGTGAACGATACCGTGCCACGTTTCCTGCACGACGGTCAGTGGTCACCCAAAGCGACTCAGGCGACGTTATCCAACGCGATGGACGTGAGTCAGCCGAACAACTGGCCGCGTGTGGAAGAGTTGTTCCGCCGCAAAATCTGGCAACTGAAAGAGCTGGGTTATGCAGCCGTGGATGATGAAACCACGCAACAGACAATGC</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>TAGCTCGGCAAACCGCCGCTACTTTTCGGTAAACAACCGCTGGAGGGATCAAATTTAGGCACGGCGTGGAAAGTGATCGGGTCTTTTTCTGCCGGTTCATAACCACGACCTTTTTTGGTCATGATATGCAGGAACTGCGGGCCTTTCAGGTCGCGCATGTTCTTTAGCGTGGTGATAAGCCCCAGCACATCGTGACCGTCCACCGGGCCGATGTAGTTAAAGCCCAGCTCTTCAAACAACGTGCCAGGCACTACCATGCCTTTAATATGTTCTTCGGTGCGTTTGAGCAGCTCTTTAATTGGCGGCACGCCAGAGAAAACTTTTTTCCCGCCTTCGCGCAGTGAAGAGTAAAGCTTACCGGAAAGCAGCTGTGCCAGATGGTTGTTGAGCGCGCCGACATTTTCGGAAATCGACATTTCATTGTCGTTGAGAATCACCAGCATATCAGGACGGATATCGCCCGCGTGATTCATCGCTTCAAACGCCATGCCTGCGGTAATCGCGCCATCGCCAATGACACAGACGGTGCGGCGATTTTTGCCTTCTTTTTCGGCAGCAACCGCAATACCAATTCCGGCACTGATGGAGGTTGATGAATGCCCGACGCTTAATACGTCATATTCGCTTTCGCCGCGCCACGGGAACGGGTGCAGACCGCCTTTCTGACGGATGGTGCCGATTTTGTCGCGGCGTCCGGTCAAAATTTTATGCGGATAAGCCTGATGCCCCACATCCCAAATCAATTGGTCAAACGGGGTGTTGTAGACATAGTGCAGCGCCACGGTCAGTTCGACCGTGCCCAGCCCGGAGGCGAAGTGCCCGCTGGAACGGCTCACGCTGTCGAGTAAATAGCGGCGCAGTTCGTCGCAGAGTTTCGGTAAACTCTCTTTCGGCAACAGTCGTAACTCCTGGGTGGAGTCGACCAGTGCCAGGGTCGGGTATTTGGCAATATCAAAACTCATCAGGGGCCTATTAATACTTATTGTTTATTTATTACGCTGGATGATGTAGTCCGCTAGCGCTTCCAGTGCCGAGGTATCGAGTGACTGTTCAGCCAGTTGTTTCAGCGACTGACGGGCATCGTCGATCAGATCCCGGGCTTTCTTCCGGGCTTGCTCAAGACCCAGAAGTGCAGGGTAGGTACTTTTACCAAGTTGCTGGTCGGCACCCTGGCGTTTT</t>
+          <t>GTACCCTCTCATGGAAGTTAGGAGTCTGACATGAAACTCTACAATCTGAAAGATCACAACGAGCAGGTCAGCTTTGCGCAAGCCGTAACCCAGGGGTTGGGCAAAAATCAGGGGCTGTTTTTTCCGCACGACCTGCCGGAATTCAGCCTGACTGAAATTGATGAGATGCTGAAGCTGGATTTTGTCACCCGCAGTGCGAAGATCCTCTCGGCGTTTATTGGTGATGAAATCCCACAGGAAATCCTGGAAGAGCGCGTGCGCGCGGCGTTTGCCTTCCCGGCTCCGGTCGCCAATGTTGAAAGCGATGTCGGTTGTCTGGAATTGTTCCACGGGCCAACGCTGGCATTTAAAGATTTCGGCGGTCGCTTTATGGCACAAATGCTGACCCATATTGCGGGTGATAAGCCAGTGACCATTCTGACCGCGACCTCCGGTGATACCGGAGCGGCAGTGGCTCATGCTTTCTACGGTTTACCGAATGTGAAAGTGGTTATCCTCTATCCACGAGGCAAAATCAGTCCACTGCAAGAAAAACTGTTCTGTACATTGGGCGGCAATATCGAAACTGTTGCCATCGACGGCGATTTCGATGCCTGTCAGGCGCTGGTGAAGCAGGCGTTTGATGATGAAGAACTGAAAGTGGCGCTAGGGTTAAACTCGGCTAACTCGATTAACATCAGCCGTTTGCTGGCGCAGATTTGCTACTACTTTGAAGCTGTTGCGCAGCTGCCGCAGGAGACGCGCAACCAGCTGGTTGTCTCGGTGCCAAGCGGAAACTTCGGCGATTTGACGGCGGGTCTGCTGGCGAAGTCACTCGGTCTGCCGGTGAAACGTTTTATTGCTGCGACCAACGTGAACGATACCGTGCCACGTTTCCTGCACGACGGTCAGTGGTCACCCAAAGCGACTCAGGCGACGTTATCCAACGCGATGGACGTGAGTCAGCCGAACAACTGGCCGCGTGTGGAAGAGTTGTTCCGCCGCAAAATCTGGCAACTGAAAGAGCTGGGTTATGCAGCCGTGGATGATGAAACCACGCAACAGACAATGCGTGAGTTAAAAGAACTGGGCTACACTTCGGAGCCGCACGCTGCCGTAGCTTATCGTGCGCTGCGTGATCAGTTGAATCCAGGCGAATATGGCTTGTTCCTCGGCACCGCGCATCCGGCGAAATTTAAAGA</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>AAACAACCGCTGGAGGGATCAAATTTAGGCACGGCGTGGAAAGTGATCGGGTCTTTTTCTGCCGGTTCATAACCACGACCTTTTTTGGTCATGATATGCAGGAACTGCGGGCCTTTCAGGTCGCGCATGTTCTTTAGCGTGGTGATAAGCCCCAGCACATCGTGACCGTCCACCGGGCCGATGTAGTTAAAGCCCAGCTCTTCAAACAACGTGCCAGGCACTACCATGCCTTTAATATGTTCTTCGGTGCGTTTGAGCAGCTCTTTAATTGGCGGCACGCCAGAGAAAACTTTTTTCCCGCCTTCGCGCAGTGAAGAGTAAAGCTTACCGGAAAGCAGCTGTGCCAGATGGTTGTTGAGCGCGCCGACATTTTCGGAAATCGACATTTCATTGTCGTTGAGAATCACCAGCATATCAGGACGGATATCGCCCGCGTGATTCATCGCTTCAAACGCCATGCCTGCGGTAATCGCGCCATCGCCAATGACACAGACGGTGCGGCGATTTTTGCCTTCTTTTTCGGCAGCAACCGCAATACCAATTCCGGCACTGATGGAGGTTGATGAATGCCCGACGCTTAATACGTCATATTCGCTTTCGCCGCGCCACGGGAACGGGTGCAGACCGCCTTTCTGACGGATGGTGCCGATTTTGTCGCGGCGTCCGGTCAAAATTTTATGCGGATAAGCCTGATGCCCCACATCCCAAATCAATTGGTCAAACGGGGTGTTGTAGACATAGTGCAGCGCCACGGTCAGTTCGACCGTGCCCAGCCCGGAGGCGAAGTGCCCGCTGGAACGGCTCACGCTGTCGAGTAAATAGCGGCGCAGTTCGTCGCAGAGTTTCGGTAAACTCTCTTTCGGCAACAGTCGTAACTCCTGGGTGGAGTCGACCAGTGCCAGGGTCGGGTATTTGGCAATATCAAAACTCATCAGGGGCCTATTAATACTTATTGTTTATTTATTACGCTGGATGATGTAGTCCGCTAGCGCTTCCAGTGCCGAGGTATCGAGTGACTG</t>
+          <t>ATGAAACTCTACAATCTGAAAGATCACAACGAGCAGGTCAGCTTTGCGCAAGCCGTAACCCAGGGGTTGGGCAAAAATCAGGGGCTGTTTTTTCCGCACGACCTGCCGGAATTCAGCCTGACTGAAATTGATGAGATGCTGAAGCTGGATTTTGTCACCCGCAGTGCGAAGATCCTCTCGGCGTTTATTGGTGATGAAATCCCACAGGAAATCCTGGAAGAGCGCGTGCGCGCGGCGTTTGCCTTCCCGGCTCCGGTCGCCAATGTTGAAAGCGATGTCGGTTGTCTGGAATTGTTCCACGGGCCAACGCTGGCATTTAAAGATTTCGGCGGTCGCTTTATGGCACAAATGCTGACCCATATTGCGGGTGATAAGCCAGTGACCATTCTGACCGCGACCTCCGGTGATACCGGAGCGGCAGTGGCTCATGCTTTCTACGGTTTACCGAATGTGAAAGTGGTTATCCTCTATCCACGAGGCAAAATCAGTCCACTGCAAGAAAAACTGTTCTGTACATTGGGCGGCAATATCGAAACTGTTGCCATCGACGGCGATTTCGATGCCTGTCAGGCGCTGGTGAAGCAGGCGTTTGATGATGAAGAACTGAAAGTGGCGCTAGGGTTAAACTCGGCTAACTCGATTAACATCAGCCGTTTGCTGGCGCAGATTTGCTACTACTTTGAAGCTGTTGCGCAGCTGCCGCAGGAGACGCGCAACCAGCTGGTTGTCTCGGTGCCAAGCGGAAACTTCGGCGATTTGACGGCGGGTCTGCTGGCGAAGTCACTCGGTCTGCCGGTGAAACGTTTTATTGCTGCGACCAACGTGAACGATACCGTGCCACGTTTCCTGCACGACGGTCAGTGGTCACCCAAAGCGACTCAGGCGACGTTATCCAACGCGATGGACGTGAGTCAGCCGAACAACTGGCCGCGTGTGGAAGAGTTGTTCCGCCGCAAAATCTGGCAACTGAAAGAGCTGGGTTATGCAGCCGTGGATGATGAAACCACGCAACAGACAATGC</t>
         </is>
       </c>
     </row>
@@ -764,35 +688,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>tktA_573_12bp_sub</t>
+          <t>b0004</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CACCTGCGCATCACTCAAAC</t>
+          <t>ATCCGTCTTGAGAATGCCCG</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CAAATAAAACGAAAGGCTCAGGTGTCGTCGGTGAACCATCCCTCGACATGACCATCGATAGAAATACCGTTGTCA</t>
+          <t>CAAATAAAACGAAAGGCTCAACGGCGGGCGCACGAGTACTGGAAAACTAAAATCTATTCATTATCTCAATCAGGC</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CAAATAAAACGAAAGGCTCAGGTGTCGTCGGTGAACCATCCCTCGACATGACCATCGATAGAAATACCGTTGTCATCGTAGAATGCAATCAGTTTACCCAGCTTCAGCGTACCCGCCAGAGAGCAAACTTCGTGGGAGATGCCTTCCATCATGCAGCCGTCGCCCATGAAGGCGTAGGTGTAGTGGTCGACAATGTCGTGGCCCGGACGGTTAAACTGCGCCGCCAGCGTTTTTTCTGCAATCGCCATACCGACTGCGTTGGCAATACCCTGACCCAGCGGACCGGTGGTGGTTTCCACACCAGCGGTGTAACCCACTTCCGGGTGACCCGGAGTTTTAGAGTGCAGCTGACGGAAGTTTTTCAGTTCTTCCATCGGCAGATCGTAACCGGTGAGGTGCAGCAGGCTGTAGATCAGCATGGAGCCGTGGCCGTTGGACAGCACGAAGCGGTCACGGTCAGCCCAGGACGGATTCTGCGGGTTGTGTTTCAGGAAATCACGCCACAGGACTTCGGCAATGTCAGCCATACCCATAGGGGCACCCGGGTGACCGGATTTGGCTTTCTGTACTGCGTCCATGCTCAGCGCACGAATAGCATTGGCAAGCTCTTTACGTGAGGACATTTTGACTCCAGATCGGATGATGAAGGGCACGCCCTTAACGACTTGACGACAGCGCGTTTTGGGCTACGCCGGAAAATTTGCCAACAATTTACCGCAAGCCGCGCGTCATGTACATGGAACATCCTTTTGCCGCTTCAGAAATCTCTGGATCATGCTCGCATGTTGCGCAATCTACTCGCCCGTCCGCTGCGCTTTTCCTTATACTGAGACTGAGCGTCGATTCACCTGCAAACGGCGCATTTTTAGAATAATCCTGACCTTGTGCGGAAGAGAAAACATGAAAATTCGCGCCTTATTGGTAGCAATGAGCGTGGCAACGGTACTGACTGGTTGCCAGAATATGGACTCCAACGGACTGCTCTCATCAGGAGCGGAAGCTTTTCAGGCTTACAGTTTGAGTGATGCGCAGGTG</t>
+          <t>CAAATAAAACGAAAGGCTCAACGGCGGGCGCACGAGTACTGGAAAACTAAAATCTATTCATTATCTCAATCAGGCCGGGTTTGCTTTTATGCAGCCCGGCTTTTTTATGAAGAAATTATGGAGAAAAATGACAGGGAAAAAGGAGAAATTCTCAATAAATGCGGTAACTTAGAGATTAGGATTGCGGAGAATAACAACCGCCGTTCTCATCGAGTAATCTCCGGATATCGACCCATAACGGGCAATGATAAAAGGAGTAACCTGTGAAAAAGATGCAATCTATCGTACTCGCACTTTCCCTGGTTCTGGTCGCTCCCATGGCAGCACAGGCTGCGGAAATTACGTTAGTCCCGTCAGTAAAATTACAGATAGGCGATCGTGATAATCGTGGCTATTACTGGGATGGAGGTCACTGGCGCGACCACGGCTGGTGGAAACAACATTATGAATGGCGAGGCAATCGCTGGCACCTACACGGACCGCCGCCACCGCCGCGCCACCATAAGAAAGCTCCTCATGATCATCACGGCGGTCATGGTCCAGGCAAACATCACCGCTAAATGACAAATGCCGGGTAACAATCCGGCATTCAGCGCCTGATGCGACGCTGGCGCGTCTTATCAGGCCTACGTTAATTCTGCAATATATTGAATCTGCATGCTTTTGTAGGCAGGATAAGGCGTTCACGCCGCATCCGGCATTGACTGCAAACTTAACGCTGCTCGTAGCGTTTAAACACCAGTTCGCCATTGCTGGAGGAATCTTCATCAAAGAAGTAACCTTCGCTATTAAAACCAGTCAGTTGCTCTGGTTTGGTCAGCCGATTTTCAATAATGAAACGACTCATCAGACCGCGTGCTTTCTTAGCGTAGAAGCTGATGATCTTAAATTTGCCGTTCTTCTCATCGAGGAACACCGGCTTGATAATCTCGGCATTCAATTTCTTCGGCTTCACCGATTTAAAATACTCATCTGACGCCAGATTAATCACCACATTATCGCCTTGTGCTGCGAGCGCCTCGTTCAGCTTGTTGGTGATGATATCTCCCCAGAATTGATACAGATCTTTCCCTCGGGCATTCTCAAGACGGAT</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1035</v>
+        <v>1093</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>GGTGTCGTCGGTGAACCATCCCTCGACATGACCATCGATAGAAATACCGTTGTCATCGTAGAATGCAATCAGTTTACCCAGCTTCAGCGTACCCGCCAGAGAGCAAACTTCGTGGGAGATGCCTTCCATCATGCAGCCGTCGCCCATGAAGGCGTAGGTGTAGTGGTCGACAATGTCGTGGCCCGGACGGTTAAACTGCGCCGCCAGCGTTTTTTCTGCAATCGCCATACCGACTGCGTTGGCAATACCCTGACCCAGCGGACCGGTGGTGGTTTCCACACCAGCGGTGTAACCCACTTCCGGGTGACCCGGAGTTTTAGAGTGCAGCTGACGGAAGTTTTTCAGTTCTTCCATCGGCAGATCGTAACCGGTGAGGTGCAGCAGGCTGTAGATCAGCATGGAGCCGTGGCCGTTGGACAGCACGAAGCGGTCACGGTCAGCCCAGGACGGATTCTGCGGGTTGTGTTTCAGGAAATCACGCCACAGGACTTCGGCAATGTCAGCCATACCCATAGGGGCACCCGGGTGACCGGATTTGGCTTTCTGTACTGCGTCCATGCTCAGCGCACGAATAGCATTGGCAAGCTCTTTACGTGAGGACATTTTGACTCCAGATCGGATGATGAAGGGCACGCCCTTAACGACTTGACGACAGCGCGTTTTGGGCTACGCCGGAAAATTTGCCAACAATTTACCGCAAGCCGCGCGTCATGTACATGGAACATCCTTTTGCCGCTTCAGAAATCTCTGGATCATGCTCGCATGTTGCGCAATCTACTCGCCCGTCCGCTGCGCTTTTCCTTATACTGAGACTGAGCGTCGATTCACCTGCAAACGGCGCATTTTTAGAATAATCCTGACCTTGTGCGGAAGAGAAAACATGAAAATTCGCGCCTTATTGGTAGCAATGAGCGTGGCAACGGTACTGACTGGTTGCCAGAATATGGACTCCAACGGACTGCTCTCATCAGGAGCGGAAGCTTTTCAGGCTTACAGTTTGAGTGATGCGCAGGTGAAAACCCTGAGCGATCAGGCATGTCAGGAGATGGACAGCAAGGCGACGATTGCGCCAGCCAATAGCGAATACGCTAAACGTCTGACAACTATTGCCAATGCGCTAGGCAACAATATCAACGGTCAGCCGG</t>
+          <t>ACGGCGGGCGCACGAGTACTGGAAAACTAAAATCTATTCATTATCTCAATCAGGCCGGGTTTGCTTTTATGCAGCCCGGCTTTTTTATGAAGAAATTATGGAGAAAAATGACAGGGAAAAAGGAGAAATTCTCAATAAATGCGGTAACTTAGAGATTAGGATTGCGGAGAATAACAACCGCCGTTCTCATCGAGTAATCTCCGGATATCGACCCATAACGGGCAATGATAAAAGGAGTAACCTGTGAAAAAGATGCAATCTATCGTACTCGCACTTTCCCTGGTTCTGGTCGCTCCCATGGCAGCACAGGCTGCGGAAATTACGTTAGTCCCGTCAGTAAAATTACAGATAGGCGATCGTGATAATCGTGGCTATTACTGGGATGGAGGTCACTGGCGCGACCACGGCTGGTGGAAACAACATTATGAATGGCGAGGCAATCGCTGGCACCTACACGGACCGCCGCCACCGCCGCGCCACCATAAGAAAGCTCCTCATGATCATCACGGCGGTCATGGTCCAGGCAAACATCACCGCTAAATGACAAATGCCGGGTAACAATCCGGCATTCAGCGCCTGATGCGACGCTGGCGCGTCTTATCAGGCCTACGTTAATTCTGCAATATATTGAATCTGCATGCTTTTGTAGGCAGGATAAGGCGTTCACGCCGCATCCGGCATTGACTGCAAACTTAACGCTGCTCGTAGCGTTTAAACACCAGTTCGCCATTGCTGGAGGAATCTTCATCAAAGAAGTAACCTTCGCTATTAAAACCAGTCAGTTGCTCTGGTTTGGTCAGCCGATTTTCAATAATGAAACGACTCATCAGACCGCGTGCTTTCTTAGCGTAGAAGCTGATGATCTTAAATTTGCCGTTCTTCTCATCGAGGAACACCGGCTTGATAATCTCGGCATTCAATTTCTTCGGCTTCACCGATTTAAAATACTCATCTGACGCCAGATTAATCACCACATTATCGCCTTGTGCTGCGAGCGCCTCGTTCAGCTTGTTGGTGATGATATCTCCCCAGAATTGATACAGATCTTTCCCTCGGGCATTCTCAAGACGGATCCCCATTTCCAGACGATAAGGCTGCATTAAATCGAGCGGGCGGAGTACGCCATACAAGCCGGAAAGCATTCGCAAATGCTGTTGGGCAAAATCGAAATCGTCTTCGCTGAAGGTTTCGGCCTGCAAGCCG</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>ACCATCGATAGAAATACCGTTGTCATCGTAGAATGCAATCAGTTTACCCAGCTTCAGCGTACCCGCCAGAGAGCAAACTTCGTGGGAGATGCCTTCCATCATGCAGCCGTCGCCCATGAAGGCGTAGGTGTAGTGGTCGACAATGTCGTGGCCCGGACGGTTAAACTGCGCCGCCAGCGTTTTTTCTGCAATCGCCATACCGACTGCGTTGGCAATACCCTGACCCAGCGGACCGGTGGTGGTTTCCACACCAGCGGTGTAACCCACTTCCGGGTGACCCGGAGTTTTAGAGTGCAGCTGACGGAAGTTTTTCAGTTCTTCCATCGGCAGATCGTAACCGGTGAGGTGCAGCAGGCTGTAGATCAGCATGGAGCCGTGGCCGTTGGACAGCACGAAGCGGTCACGGTCAGCCCAGGACGGATTCTGCGGGTTGTGTTTCAGGAAATCACGCCACAGGACTTCGGCAATGTCAGCCATACCCATAGGGGCACCCGGGTGACCGGATTTGGCTTTCTGTACTGCGTCCATGCTCAGCGCACGAATAGCATTGGCAAGCTCTTTACGTGAGGACATTTTGACTCCAGATCGGATGATGAAGGGCACGCCCTTAACGACTTGACGACAGCGCGTTTTGGGCTACGCCGGAAAATTTGCCAACAATTTACCGCAAGCCGCGCGTCATGTACATGGAACATCCTTTTGCCGCTTCAGAAATCTCTGGATCATGCTCGCATGTTGCGCAATCTACTCGCCCGTCCGCTGCGCTTTTCCTTATACTGAGACTGAGCGTCGATTCACCTGCAAACGGCGCATTTTTAGAATAATCCTGACCTTGTGCGGAAGAGAAAACATGAAAATTCGCGCCTTATTGGTAGCAATGAGCGTGGCAACGGTACTGACTGGTTGCCAGAATATGGACTCCAACGGACTGCTCTCATCAGGAGCGGAAGCTTTTCAGGCTTACAGTTTGAGTGATGCGCAGGTG</t>
+          <t>AATCTATTCATTATCTCAATCAGGCCGGGTTTGCTTTTATGCAGCCCGGCTTTTTTATGAAGAAATTATGGAGAAAAATGACAGGGAAAAAGGAGAAATTCTCAATAAATGCGGTAACTTAGAGATTAGGATTGCGGAGAATAACAACCGCCGTTCTCATCGAGTAATCTCCGGATATCGACCCATAACGGGCAATGATAAAAGGAGTAACCTGTGAAAAAGATGCAATCTATCGTACTCGCACTTTCCCTGGTTCTGGTCGCTCCCATGGCAGCACAGGCTGCGGAAATTACGTTAGTCCCGTCAGTAAAATTACAGATAGGCGATCGTGATAATCGTGGCTATTACTGGGATGGAGGTCACTGGCGCGACCACGGCTGGTGGAAACAACATTATGAATGGCGAGGCAATCGCTGGCACCTACACGGACCGCCGCCACCGCCGCGCCACCATAAGAAAGCTCCTCATGATCATCACGGCGGTCATGGTCCAGGCAAACATCACCGCTAAATGACAAATGCCGGGTAACAATCCGGCATTCAGCGCCTGATGCGACGCTGGCGCGTCTTATCAGGCCTACGTTAATTCTGCAATATATTGAATCTGCATGCTTTTGTAGGCAGGATAAGGCGTTCACGCCGCATCCGGCATTGACTGCAAACTTAACGCTGCTCGTAGCGTTTAAACACCAGTTCGCCATTGCTGGAGGAATCTTCATCAAAGAAGTAACCTTCGCTATTAAAACCAGTCAGTTGCTCTGGTTTGGTCAGCCGATTTTCAATAATGAAACGACTCATCAGACCGCGTGCTTTCTTAGCGTAGAAGCTGATGATCTTAAATTTGCCGTTCTTCTCATCGAGGAACACCGGCTTGATAATCTCGGCATTCAATTTCTTCGGCTTCACCGATTTAAAATACTCATCTGACGCCAGATTAATCACCACATTATCGCCTTGTGCTGCGAGCGCCTCGTTCAGCTTGTTGGTGATGATATCTCCCCAGAATTGATACAGATCTTTCCCTCGGGCATTCTCAAGACGGAT</t>
         </is>
       </c>
     </row>
@@ -802,111 +726,35 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>aceE_del</t>
+          <t>b0005</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>TTAACACCAAACTCGCGTGC</t>
+          <t>GACGCGTGGGATGATGTTTC</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CAAATAAAACGAAAGGCTCACAACGTTATTAGATAGATAAGGAATAACCCGAGGTAAAAGAATAATGGCTATCGA</t>
+          <t>CAAATAAAACGAAAGGCTCACATAACGGGCAATGATAAAAGGAGTAACCTATGACAAATGCCGGGTAACA</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CAAATAAAACGAAAGGCTCACAACGTTATTAGATAGATAAGGAATAACCCGAGGTAAAAGAATAATGGCTATCGAAATCAAAGTACCGGACATCGGGGCTGATGAAGTTGAAATCACCGAGATCCTGGTCAAAGTGGGCGACAAAGTTGAAGCCGAACAGTCGCTGATCACCGTAGAAGGCGACAAAGCCTCTATGGAAGTTCCGTCTCCGCAGGCGGGTATCGTTAAAGAGATCAAAGTCTCTGTTGGCGATAAAACCCAGACCGGCGCACTGATTATGATTTTCGATTCCGCCGACGGTGCAGCAGACGCTGCACCTGCTCAGGCAGAAGAGAAGAAAGAAGCAGCTCCGGCAGCAGCACCAGCGGCTGCGGCGGCAAAAGACGTTAACGTTCCGGATATCGGCAGCGACGAAGTTGAAGTGACCGAAATCCTGGTGAAAGTTGGCGATAAAGTTGAAGCTGAACAGTCGCTGATCACCGTAGAAGGCGACAAGGCTTCTATGGAAGTTCCGGCTCCGTTTGCTGGCACCGTGAAAGAGATCAAAGTGAACGTGGGTGACAAAGTGTCTACCGGCTCGCTGATTATGGTCTTCGAAGTCGCGGGTGAAGCAGGCGCGGCAGCTCCGGCCGCTAAACAGGAAGCAGCTCCGGCAGCGGCCCCTGCACCAGCGGCTGGCGTGAAAGAAGTTAACGTTCCGGATATCGGCGGTGACGAAGTTGAAGTGACTGAAGTGATGGTGAAAGTGGGCGACAAAGTTGCCGCTGAACAGTCACTGATCACCGTAGAAGGCGACAAAGCTTCTATGGAAGTTCCGGCGCCGTTTGCAGGCGTCGTGAAGGAACTGAAAGTCAACGTTGGCGATAAAGTGAAAACTGGCTCGCTGATTATGATCTTCGAAGTTGAAGGCGCAGCGCCTGCGGCAGCTCCTGCGAAACAGGAAGCGGCAGCGCCGGCACCGGCAGCAAAAGCTGAAGCCCCGGCAGCAGCACCAGCTGCGAAAGCGGAAGGCAAATCTGAATTTGCTGAAAACGACGCTTATGTTCACGCGACTCCGCTGATCCGCCGTCTGGCACGCGAGTTTGGTGTTAA</t>
+          <t>CAAATAAAACGAAAGGCTCACATAACGGGCAATGATAAAAGGAGTAACCTATGACAAATGCCGGGTAACAATCCGGCATTCAGCGCCTGATGCGACGCTGGCGCGTCTTATCAGGCCTACGTTAATTCTGCAATATATTGAATCTGCATGCTTTTGTAGGCAGGATAAGGCGTTCACGCCGCATCCGGCATTGACTGCAAACTTAACGCTGCTCGTAGCGTTTAAACACCAGTTCGCCATTGCTGGAGGAATCTTCATCAAAGAAGTAACCTTCGCTATTAAAACCAGTCAGTTGCTCTGGTTTGGTCAGCCGATTTTCAATAATGAAACGACTCATCAGACCGCGTGCTTTCTTAGCGTAGAAGCTGATGATCTTAAATTTGCCGTTCTTCTCATCGAGGAACACCGGCTTGATAATCTCGGCATTCAATTTCTTCGGCTTCACCGATTTAAAATACTCATCTGACGCCAGATTAATCACCACATTATCGCCTTGTGCTGCGAGCGCCTCGTTCAGCTTGTTGGTGATGATATCTCCCCAGAATTGATACAGATCTTTCCCTCGGGCATTCTCAAGACGGATCCCCATTTCCAGACGATAAGGCTGCATTAAATCGAGCGGGCGGAGTACGCCATACAAGCCGGAAAGCATTCGCAAATGCTGTTGGGCAAAATCGAAATCGTCTTCGCTGAAGGTTTCGGCCTGCAAGCCGGTGTAGACATCACCTTTAAACGCCAGAATCGCCTGGCGGGCATTCGCCGGCGTGAAATCTGGCTGCCAGTCATGAAAGCGAGCGGCGTTGATACCCGCCAGTTTGTCGCTGATGCGCATCAGCGTGCTAATCTGCGGAGGCGTCAGTTTCCGCGCCTCATGGATCAACTGCTGGGAATTGTCTAACAGCTCCGGCAGCGTATAGCGCGTGGTGGTCAACGGGCTTTGGTAATCAAGCGTTTTCGCAGGTGAAATAAGAATCAGCATATCCAGTCCTTGCAGGAAATTTATGCCGACTTTAGCAAAAAATGAGAATGAGTTGATCGATAGTTGTGATTACTCCTGCGAAACATCATCCCACGCGTC</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1092</v>
+        <v>1078</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>CAACGTTATTAGATAGATAAGGAATAACCCGAGGTAAAAGAATAATGGCTATCGAAATCAAAGTACCGGACATCGGGGCTGATGAAGTTGAAATCACCGAGATCCTGGTCAAAGTGGGCGACAAAGTTGAAGCCGAACAGTCGCTGATCACCGTAGAAGGCGACAAAGCCTCTATGGAAGTTCCGTCTCCGCAGGCGGGTATCGTTAAAGAGATCAAAGTCTCTGTTGGCGATAAAACCCAGACCGGCGCACTGATTATGATTTTCGATTCCGCCGACGGTGCAGCAGACGCTGCACCTGCTCAGGCAGAAGAGAAGAAAGAAGCAGCTCCGGCAGCAGCACCAGCGGCTGCGGCGGCAAAAGACGTTAACGTTCCGGATATCGGCAGCGACGAAGTTGAAGTGACCGAAATCCTGGTGAAAGTTGGCGATAAAGTTGAAGCTGAACAGTCGCTGATCACCGTAGAAGGCGACAAGGCTTCTATGGAAGTTCCGGCTCCGTTTGCTGGCACCGTGAAAGAGATCAAAGTGAACGTGGGTGACAAAGTGTCTACCGGCTCGCTGATTATGGTCTTCGAAGTCGCGGGTGAAGCAGGCGCGGCAGCTCCGGCCGCTAAACAGGAAGCAGCTCCGGCAGCGGCCCCTGCACCAGCGGCTGGCGTGAAAGAAGTTAACGTTCCGGATATCGGCGGTGACGAAGTTGAAGTGACTGAAGTGATGGTGAAAGTGGGCGACAAAGTTGCCGCTGAACAGTCACTGATCACCGTAGAAGGCGACAAAGCTTCTATGGAAGTTCCGGCGCCGTTTGCAGGCGTCGTGAAGGAACTGAAAGTCAACGTTGGCGATAAAGTGAAAACTGGCTCGCTGATTATGATCTTCGAAGTTGAAGGCGCAGCGCCTGCGGCAGCTCCTGCGAAACAGGAAGCGGCAGCGCCGGCACCGGCAGCAAAAGCTGAAGCCCCGGCAGCAGCACCAGCTGCGAAAGCGGAAGGCAAATCTGAATTTGCTGAAAACGACGCTTATGTTCACGCGACTCCGCTGATCCGCCGTCTGGCACGCGAGTTTGGTGTTAACCTTGCGAAAGTGAAGGGCACTGGCCGTAAAGGTCGTATCCTGCGCGAAGACGTTCAGGCTTACGTGAAAGAAGCTATCAAACGTGCAGAAGCAGCTCCGGCAGCGACTGGCGGTGGTATCCCTGGCATG</t>
+          <t>CATAACGGGCAATGATAAAAGGAGTAACCTATGACAAATGCCGGGTAACAATCCGGCATTCAGCGCCTGATGCGACGCTGGCGCGTCTTATCAGGCCTACGTTAATTCTGCAATATATTGAATCTGCATGCTTTTGTAGGCAGGATAAGGCGTTCACGCCGCATCCGGCATTGACTGCAAACTTAACGCTGCTCGTAGCGTTTAAACACCAGTTCGCCATTGCTGGAGGAATCTTCATCAAAGAAGTAACCTTCGCTATTAAAACCAGTCAGTTGCTCTGGTTTGGTCAGCCGATTTTCAATAATGAAACGACTCATCAGACCGCGTGCTTTCTTAGCGTAGAAGCTGATGATCTTAAATTTGCCGTTCTTCTCATCGAGGAACACCGGCTTGATAATCTCGGCATTCAATTTCTTCGGCTTCACCGATTTAAAATACTCATCTGACGCCAGATTAATCACCACATTATCGCCTTGTGCTGCGAGCGCCTCGTTCAGCTTGTTGGTGATGATATCTCCCCAGAATTGATACAGATCTTTCCCTCGGGCATTCTCAAGACGGATCCCCATTTCCAGACGATAAGGCTGCATTAAATCGAGCGGGCGGAGTACGCCATACAAGCCGGAAAGCATTCGCAAATGCTGTTGGGCAAAATCGAAATCGTCTTCGCTGAAGGTTTCGGCCTGCAAGCCGGTGTAGACATCACCTTTAAACGCCAGAATCGCCTGGCGGGCATTCGCCGGCGTGAAATCTGGCTGCCAGTCATGAAAGCGAGCGGCGTTGATACCCGCCAGTTTGTCGCTGATGCGCATCAGCGTGCTAATCTGCGGAGGCGTCAGTTTCCGCGCCTCATGGATCAACTGCTGGGAATTGTCTAACAGCTCCGGCAGCGTATAGCGCGTGGTGGTCAACGGGCTTTGGTAATCAAGCGTTTTCGCAGGTGAAATAAGAATCAGCATATCCAGTCCTTGCAGGAAATTTATGCCGACTTTAGCAAAAAATGAGAATGAGTTGATCGATAGTTGTGATTACTCCTGCGAAACATCATCCCACGCGTCCGGAGAAAGCTGGCGACCGATATCCGGATAACGCAATGGATCAAACACCGGGCGCACGCCGAGTTTACGCTGGCGTAGATAATCACTGGCAATGGTATGAACCACAGGCGAGAGCAGTAAAATGGCGGTC</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>GAGGTAAAAGAATAATGGCTATCGAAATCAAAGTACCGGACATCGGGGCTGATGAAGTTGAAATCACCGAGATCCTGGTCAAAGTGGGCGACAAAGTTGAAGCCGAACAGTCGCTGATCACCGTAGAAGGCGACAAAGCCTCTATGGAAGTTCCGTCTCCGCAGGCGGGTATCGTTAAAGAGATCAAAGTCTCTGTTGGCGATAAAACCCAGACCGGCGCACTGATTATGATTTTCGATTCCGCCGACGGTGCAGCAGACGCTGCACCTGCTCAGGCAGAAGAGAAGAAAGAAGCAGCTCCGGCAGCAGCACCAGCGGCTGCGGCGGCAAAAGACGTTAACGTTCCGGATATCGGCAGCGACGAAGTTGAAGTGACCGAAATCCTGGTGAAAGTTGGCGATAAAGTTGAAGCTGAACAGTCGCTGATCACCGTAGAAGGCGACAAGGCTTCTATGGAAGTTCCGGCTCCGTTTGCTGGCACCGTGAAAGAGATCAAAGTGAACGTGGGTGACAAAGTGTCTACCGGCTCGCTGATTATGGTCTTCGAAGTCGCGGGTGAAGCAGGCGCGGCAGCTCCGGCCGCTAAACAGGAAGCAGCTCCGGCAGCGGCCCCTGCACCAGCGGCTGGCGTGAAAGAAGTTAACGTTCCGGATATCGGCGGTGACGAAGTTGAAGTGACTGAAGTGATGGTGAAAGTGGGCGACAAAGTTGCCGCTGAACAGTCACTGATCACCGTAGAAGGCGACAAAGCTTCTATGGAAGTTCCGGCGCCGTTTGCAGGCGTCGTGAAGGAACTGAAAGTCAACGTTGGCGATAAAGTGAAAACTGGCTCGCTGATTATGATCTTCGAAGTTGAAGGCGCAGCGCCTGCGGCAGCTCCTGCGAAACAGGAAGCGGCAGCGCCGGCACCGGCAGCAAAAGCTGAAGCCCCGGCAGCAGCACCAGCTGCGAAAGCGGAAGGCAAATCTGAATTTGCTGAAAACGACGCTTATGTTCACGCGACTCCGCTGATCCGCCGTCTGGCACGCGAGTTTGGTGTTAA</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>pntA_promoter_sub</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ACTTGGTGATGCGGTAGTCG</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CAAATAAAACGAAAGGCTCACTAGATTCGTGCTAGCATTATACCTAGGACTGAGCTAGCTGTCAAGGCGCGGTGATAGTGGGATAAACACCT</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>CAAATAAAACGAAAGGCTCACTAGATTCGTGCTAGCATTATACCTAGGACTGAGCTAGCTGTCAAGGCGCGGTGATAGTGGGATAAACACCTTAGAACGCCGGATAAAGACTGATAATTGTCTTCGACGGTCGGGTAAAACGAGACATCGCCCCGGCACGAATCACTACTTAACATTAAATTAACTTATACAATTCAGTTGCTTCAGTAGTAATGATGCTGATACGGCTGTTTTTTAAGCATAGACGGTCATTTGAGCAGGATTAAAATTGGCTTAAGGAATGTGATATGAAAAATGACGCAGACAGTTACACCGTTTAAATGCAATAATCAGCCACGTTTCTCGTTAATAACAATACCAGTACCTGGTTTGCGCAAGGCGAAGGATTATTTTTATGAAGCTTAAGAACACCCTCCTGGCGTCGGCACTGCTTTCTGCTATGGCATTCTCCGTTAACGCAGCAACAGAACTGACACCGGAGCAAGCGGCAGCGGTTAAACCTTTTGACCGTGTAGTGGTTACCGGTCGTTTTAATGCTATTGGCGAAGCGGTGAAAGCCGTTTCTCGTCGCGCAGATAAAGAAGGTGCCGCCTCTTTTTATGTTGTCGACACTTCTGATTTTGGTAACAGCGGTAACTGGCGTGTGGTCGCTGACCTCTATAAAGCCGATGCTGAAAAAGCAGAAGAAACAAGTAATCGCGTAATTAACGGTGTTGTCGAACTGCCGAAAGATCAGGCTGTTCTGATTGAACCGTTTGACACGGTCACCGTCCAGGGCTTCTATCGTAGCCAGCCAGAAGTCAATGATGCCATCACCAAAGCGGCAAAAGCGAAAGGTGCCTACTCTTTCTACATCGTTCGTCAAATCGATGCCAACCAGGGCGGCAACCAGCGTATTACTGCATTCATCTATAAAAAAGATGCTAAGAAACGTATCGTCCAGAGCCCGGATGTGATCCCGGCAGATTCCGAAGCAGGACGTGCAGCTCTGGCTGCCGGTGGCGAAGCCGCGAAGAAAGTTGAGATCCCGGGTGTTGCGACTACCGCATCACCAAGT</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>1057</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>CTAGATTCGTGCTAGCATTATACCTAGGACTGAGCTAGCTGTCAAGGCGCGGTGATAGTGGGATAAACACCTTAGAACGCCGGATAAAGACTGATAATTGTCTTCGACGGTCGGGTAAAACGAGACATCGCCCCGGCACGAATCACTACTTAACATTAAATTAACTTATACAATTCAGTTGCTTCAGTAGTAATGATGCTGATACGGCTGTTTTTTAAGCATAGACGGTCATTTGAGCAGGATTAAAATTGGCTTAAGGAATGTGATATGAAAAATGACGCAGACAGTTACACCGTTTAAATGCAATAATCAGCCACGTTTCTCGTTAATAACAATACCAGTACCTGGTTTGCGCAAGGCGAAGGATTATTTTTATGAAGCTTAAGAACACCCTCCTGGCGTCGGCACTGCTTTCTGCTATGGCATTCTCCGTTAACGCAGCAACAGAACTGACACCGGAGCAAGCGGCAGCGGTTAAACCTTTTGACCGTGTAGTGGTTACCGGTCGTTTTAATGCTATTGGCGAAGCGGTGAAAGCCGTTTCTCGTCGCGCAGATAAAGAAGGTGCCGCCTCTTTTTATGTTGTCGACACTTCTGATTTTGGTAACAGCGGTAACTGGCGTGTGGTCGCTGACCTCTATAAAGCCGATGCTGAAAAAGCAGAAGAAACAAGTAATCGCGTAATTAACGGTGTTGTCGAACTGCCGAAAGATCAGGCTGTTCTGATTGAACCGTTTGACACGGTCACCGTCCAGGGCTTCTATCGTAGCCAGCCAGAAGTCAATGATGCCATCACCAAAGCGGCAAAAGCGAAAGGTGCCTACTCTTTCTACATCGTTCGTCAAATCGATGCCAACCAGGGCGGCAACCAGCGTATTACTGCATTCATCTATAAAAAAGATGCTAAGAAACGTATCGTCCAGAGCCCGGATGTGATCCCGGCAGATTCCGAAGCAGGACGTGCAGCTCTGGCTGCCGGTGGCGAAGCCGCGAAGAAAGTTGAGATCCCGGGTGTTGCGACTACCGCATCACCAAGTTCTGAAGTCGGTCGCTTCTTTGAAACCCAGTCATCAAAAGGCGGGCGTTACACCGTCACGCTCCCGGATGGCACTAAAGTCGAAGAACTGAACAAAGCGACCGCAGCGATGATGGTCCCGTTCGACAGCA</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>GTGATAGTGGGATAAACACCTTAGAACGCCGGATAAAGACTGATAATTGTCTTCGACGGTCGGGTAAAACGAGACATCGCCCCGGCACGAATCACTACTTAACATTAAATTAACTTATACAATTCAGTTGCTTCAGTAGTAATGATGCTGATACGGCTGTTTTTTAAGCATAGACGGTCATTTGAGCAGGATTAAAATTGGCTTAAGGAATGTGATATGAAAAATGACGCAGACAGTTACACCGTTTAAATGCAATAATCAGCCACGTTTCTCGTTAATAACAATACCAGTACCTGGTTTGCGCAAGGCGAAGGATTATTTTTATGAAGCTTAAGAACACCCTCCTGGCGTCGGCACTGCTTTCTGCTATGGCATTCTCCGTTAACGCAGCAACAGAACTGACACCGGAGCAAGCGGCAGCGGTTAAACCTTTTGACCGTGTAGTGGTTACCGGTCGTTTTAATGCTATTGGCGAAGCGGTGAAAGCCGTTTCTCGTCGCGCAGATAAAGAAGGTGCCGCCTCTTTTTATGTTGTCGACACTTCTGATTTTGGTAACAGCGGTAACTGGCGTGTGGTCGCTGACCTCTATAAAGCCGATGCTGAAAAAGCAGAAGAAACAAGTAATCGCGTAATTAACGGTGTTGTCGAACTGCCGAAAGATCAGGCTGTTCTGATTGAACCGTTTGACACGGTCACCGTCCAGGGCTTCTATCGTAGCCAGCCAGAAGTCAATGATGCCATCACCAAAGCGGCAAAAGCGAAAGGTGCCTACTCTTTCTACATCGTTCGTCAAATCGATGCCAACCAGGGCGGCAACCAGCGTATTACTGCATTCATCTATAAAAAAGATGCTAAGAAACGTATCGTCCAGAGCCCGGATGTGATCCCGGCAGATTCCGAAGCAGGACGTGCAGCTCTGGCTGCCGGTGGCGAAGCCGCGAAGAAAGTTGAGATCCCGGGTGTTGCGACTACCGCATCACCAAGT</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Cgl1452_ins</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CGATGTCGCTGGCGTTAATG</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>CAAATAAAACGAAAGGCTCATCCGGCGACCGCTCCGAGGTTGAAGCTTAAGCATCCGGCATGAACAAAGC</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>CAAATAAAACGAAAGGCTCATCCGGCGACCGCTCCGAGGTTGAAGCTTAAGCATCCGGCATGAACAAAGCGTACTTTGCTTAATTCAGGCTGGAACGTGGCGATGACCCAGCAAAGATAAAACGAGTCACAGGTTATGCATGAGAGGAAATCAGGCGCTTCGCCGCTATTTCGAATTTATTCCATTGCCCGATACACGGCCTCGCCAATTTGCTTCAGTGCTTCGCGATAGGTTTCGCTGAGCGGCAAAGCGCAGTTGATGCGCAGACAATTACGGTATTTGCCGGAAGCTGAGAAAATCGAGCCTGCCGCCACCTGGATTTTCATGCGGCACAGCTGCCGCGCGACGCAGACCATATCGACCTGTTCAGGCAATTCTATCCACAGTAAAAATCCGCCTTTCGGGCGCGTAATACAGATTTCGCAGGGAAAATATTCCCGTATCCAGCAGGTATAAAGCGCCAAATTGCGCTGATAGATCTGCCGCATCCGCCGGATATGGCGATGATAGTGACCTTCCAGCACAAACGTTGCCGCCGCCATTTGCGTGGACGGCACATTAAAGCTGCTGATGGCGTATTTCATATGCATCAGTTTATCGTGATAACGCCCCGGTGCGACCCAACCCACGCGCAGGCCTGGTGCAATACTTTTACTGAACGAGCTGCACAACAGCACTCGCCCGTCGATATCCCAGGAATGAATGGTCCGCGGGCGCGGATACTCCGTCGCCAGTTCGCCATAGACATCATCTTCAAAAATCACAATATCATGACGCTGAGCGAGAGAGAGAACGGCCCGTTTGCGCGCGTCCGGCATAATAAATCCCAGCGGATTATTACAGTTTGGCACCAGAATGATGCCTTTAATCGGCCACTGTTCCAGCGCCAGTTCCAGCGCTTCAACGCTGATGCCAGTTTCTGGATCGGTTGGGATTTCAATCACTTTCACGCCCATGCCGCGCAGCATCTGCATCGAACCGTAATAACAGGGGGATTCGACCGCGACAATATCGCCCGGTTTACACACTGCCATTAACGCCAGCGACATCG</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>1051</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>TCCGGCGACCGCTCCGAGGTTGAAGCTTAAGCATCCGGCATGAACAAAGCGTACTTTGCTTAATTCAGGCTGGAACGTGGCGATGACCCAGCAAAGATAAAACGAGTCACAGGTTATGCATGAGAGGAAATCAGGCGCTTCGCCGCTATTTCGAATTTATTCCATTGCCCGATACACGGCCTCGCCAATTTGCTTCAGTGCTTCGCGATAGGTTTCGCTGAGCGGCAAAGCGCAGTTGATGCGCAGACAATTACGGTATTTGCCGGAAGCTGAGAAAATCGAGCCTGCCGCCACCTGGATTTTCATGCGGCACAGCTGCCGCGCGACGCAGACCATATCGACCTGTTCAGGCAATTCTATCCACAGTAAAAATCCGCCTTTCGGGCGCGTAATACAGATTTCGCAGGGAAAATATTCCCGTATCCAGCAGGTATAAAGCGCCAAATTGCGCTGATAGATCTGCCGCATCCGCCGGATATGGCGATGATAGTGACCTTCCAGCACAAACGTTGCCGCCGCCATTTGCGTGGACGGCACATTAAAGCTGCTGATGGCGTATTTCATATGCATCAGTTTATCGTGATAACGCCCCGGTGCGACCCAACCCACGCGCAGGCCTGGTGCAATACTTTTACTGAACGAGCTGCACAACAGCACTCGCCCGTCGATATCCCAGGAATGAATGGTCCGCGGGCGCGGATACTCCGTCGCCAGTTCGCCATAGACATCATCTTCAAAAATCACAATATCATGACGCTGAGCGAGAGAGAGAACGGCCCGTTTGCGCGCGTCCGGCATAATAAATCCCAGCGGATTATTACAGTTTGGCACCAGAATGATGCCTTTAATCGGCCACTGTTCCAGCGCCAGTTCCAGCGCTTCAACGCTGATGCCAGTTTCTGGATCGGTTGGGATTTCAATCACTTTCACGCCCATGCCGCGCAGCATCTGCATCGAACCGTAATAACAGGGGGATTCGACCGCGACAATATCGCCCGGTTTACACACTGCCATTAACGCCAGCGACATCGAGTTATGGCAGCCGCTGGTGATGATGATGTCATCGGCGGTGACCACCGAGCCGCTGTCGAGCATCAGGCGGGCAATCTGCTCTCGCAATACTCGCTGACCGGCTAACAAGTCATAACCGAGAACGGTTTG</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>GCATCCGGCATGAACAAAGCGTACTTTGCTTAATTCAGGCTGGAACGTGGCGATGACCCAGCAAAGATAAAACGAGTCACAGGTTATGCATGAGAGGAAATCAGGCGCTTCGCCGCTATTTCGAATTTATTCCATTGCCCGATACACGGCCTCGCCAATTTGCTTCAGTGCTTCGCGATAGGTTTCGCTGAGCGGCAAAGCGCAGTTGATGCGCAGACAATTACGGTATTTGCCGGAAGCTGAGAAAATCGAGCCTGCCGCCACCTGGATTTTCATGCGGCACAGCTGCCGCGCGACGCAGACCATATCGACCTGTTCAGGCAATTCTATCCACAGTAAAAATCCGCCTTTCGGGCGCGTAATACAGATTTCGCAGGGAAAATATTCCCGTATCCAGCAGGTATAAAGCGCCAAATTGCGCTGATAGATCTGCCGCATCCGCCGGATATGGCGATGATAGTGACCTTCCAGCACAAACGTTGCCGCCGCCATTTGCGTGGACGGCACATTAAAGCTGCTGATGGCGTATTTCATATGCATCAGTTTATCGTGATAACGCCCCGGTGCGACCCAACCCACGCGCAGGCCTGGTGCAATACTTTTACTGAACGAGCTGCACAACAGCACTCGCCCGTCGATATCCCAGGAATGAATGGTCCGCGGGCGCGGATACTCCGTCGCCAGTTCGCCATAGACATCATCTTCAAAAATCACAATATCATGACGCTGAGCGAGAGAGAGAACGGCCCGTTTGCGCGCGTCCGGCATAATAAATCCCAGCGGATTATTACAGTTTGGCACCAGAATGATGCCTTTAATCGGCCACTGTTCCAGCGCCAGTTCCAGCGCTTCAACGCTGATGCCAGTTTCTGGATCGGTTGGGATTTCAATCACTTTCACGCCCATGCCGCGCAGCATCTGCATCGAACCGTAATAACAGGGGGATTCGACCGCGACAATATCGCCCGGTTTACACACTGCCATTAACGCCAGCGACATCG</t>
+          <t>ATGACAAATGCCGGGTAACAATCCGGCATTCAGCGCCTGATGCGACGCTGGCGCGTCTTATCAGGCCTACGTTAATTCTGCAATATATTGAATCTGCATGCTTTTGTAGGCAGGATAAGGCGTTCACGCCGCATCCGGCATTGACTGCAAACTTAACGCTGCTCGTAGCGTTTAAACACCAGTTCGCCATTGCTGGAGGAATCTTCATCAAAGAAGTAACCTTCGCTATTAAAACCAGTCAGTTGCTCTGGTTTGGTCAGCCGATTTTCAATAATGAAACGACTCATCAGACCGCGTGCTTTCTTAGCGTAGAAGCTGATGATCTTAAATTTGCCGTTCTTCTCATCGAGGAACACCGGCTTGATAATCTCGGCATTCAATTTCTTCGGCTTCACCGATTTAAAATACTCATCTGACGCCAGATTAATCACCACATTATCGCCTTGTGCTGCGAGCGCCTCGTTCAGCTTGTTGGTGATGATATCTCCCCAGAATTGATACAGATCTTTCCCTCGGGCATTCTCAAGACGGATCCCCATTTCCAGACGATAAGGCTGCATTAAATCGAGCGGGCGGAGTACGCCATACAAGCCGGAAAGCATTCGCAAATGCTGTTGGGCAAAATCGAAATCGTCTTCGCTGAAGGTTTCGGCCTGCAAGCCGGTGTAGACATCACCTTTAAACGCCAGAATCGCCTGGCGGGCATTCGCCGGCGTGAAATCTGGCTGCCAGTCATGAAAGCGAGCGGCGTTGATACCCGCCAGTTTGTCGCTGATGCGCATCAGCGTGCTAATCTGCGGAGGCGTCAGTTTCCGCGCCTCATGGATCAACTGCTGGGAATTGTCTAACAGCTCCGGCAGCGTATAGCGCGTGGTGGTCAACGGGCTTTGGTAATCAAGCGTTTTCGCAGGTGAAATAAGAATCAGCATATCCAGTCCTTGCAGGAAATTTATGCCGACTTTAGCAAAAAATGAGAATGAGTTGATCGATAGTTGTGATTACTCCTGCGAAACATCATCCCACGCGTC</t>
         </is>
       </c>
     </row>
@@ -921,7 +769,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -987,41 +835,41 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dxs_sub_933_C_T_sub</t>
+          <t>b0003</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>AACGCGAAGGTCGGTTTTTCCTAAGGGGTTGTATTGCATGCTGCCACTCCTGCTATACTCGTCATACTTCAAGTTGCATGTGCTGCGGCTGCATTCGTTCACCCCAGTCACTTACTTATGTAAGCTCCTGGGGCTTCACTCGTTTGCCGCCTTCCTGCAACTCGAATTATTTAGAGTCTATGAATAATTTCTTAAGCATAGCAGGAGTGGAGTAGGGATTATGCCAGCCAGGCCTTGATTTTGGCTTCCATACCAGCGGCATCGAGGCCGAGTTCGGCGCGCATTTCTTCCTGAGTTCCTTGCGGAATAAAGAAGTCCGGCAGGCCAATGTTCAGCACGGGTACTGGTTTACGATGGGCCATCAGCACTTCGTTCACGCCGCTGCCTGCGCCGCCCATAATGGCGTTTTCTTCTACGGTGACCAGCGCTTCATGGCTGGCGGCCATTTCCAGAATTAACGCTTCATCAAGCGGTTTCACAAAACGCATATCGACCAGCGTGGCGTTCAGCGATTCGGCGACTTTCGCCGCTTCTGGCATCAGCGTACCAAAGTTAAGGATCGCCAGTTTCTCGCCACGACGCTTCACAATGCCTTTGCCAATTGGTAGTTTTTCCAGCGGCGTCAGTTCCACGCCGACCGCGTTGCCACGCGGGTAGCGCACCGCTGACGGGCCATCGTTATAGTGATAGCCGGTATAGAGCATCTGGCGACATTCGTTTTCATCGCTCGGGGTCATAATGACCATTTCCGGTATGCAGCGCAGGTAAGAGAGATCAAAAGCACCCTGATGGGTTTGACCGTCAGCACCAACAATGCCCGCGCGGTCGATGGCGAACAGGACCGGAAGCTTTTGAATCGCCACGTCATGCAGCACCTGATCATAGGCGCGTTGCAGGAAAGTGGAGTAAATCGCGACAATGGGTTTGTACCCACCAATCGCCAGACCCGCAGCAAAGGTCACCGCGTGTTGCTCGGCAATTGCCACGTCGAAGTAGCGATCCGGGAATTTACGTGAAAACTCGACCATGCCGGAACCTTCACGCATCGCCGGAGTAATCGCCATCAGCTTGTTGTCTTTCGCTGCCGTTTCGCACAACCAGTCGCCAAAGATTTTTGAATAGCTCGGCAAACCGCCGCTACTTTTCGGTAGCTCGGCAAACCGCCGCTACTTTTCGGTAAACAACCGCTGGAGGGATCAAATTTAGGCACGGCGTGGAAAGTGATCGGGTCTTTTTCTGCCGGTTCATAACCACGACCTTTTTTGGTCATGATATGCAGGAACTGCGGGCCTTTCAGGTCGCGCATGTTCTTTAGCGTGGTGATAAGCCCCAGCACATCGTGACCGTCCACCGGGCCGATGTAGTTAAAGCCCAGCTCTTCAAACAACGTGCCAGGCACTACCATGCCTTTAATATGTTCTTCGGTGCGTTTGAGCAGCTCTTTAATTGGCGGCACGCCAGAGAAAACTTTTTTCCCGCCTTCGCGCAGTGAAGAGTAAAGCTTACCGGAAAGCAGCTGTGCCAGATGGTTGTTGAGCGCGCCGACATTTTCGGAAATCGACATTTCATTGTCGTTGAGAATCACCAGCATATCAGGACGGATATCGCCCGCGTGATTCATCGCTTCAAACGCCATGCCTGCGGTAATCGCGCCATCGCCAATGACACAGACGGTGCGGCGATTTTTGCCTTCTTTTTCGGCAGCAACCGCAATACCAATTCCGGCACTGATGGAGGTTGATGAATGCCCGACGCTTAATACGTCATATTCGCTTTCGCCGCGCCACGGGAACGGGTGCAGACCGCCTTTCTGACGGATGGTGCCGATTTTGTCGCGGCGTCCGGTCAAAATTTTATGCGGATAAGCCTGATGCCCCACATCCCAAATCAATTGGTCAAACGGGGTGTTGTAGACATAGTGCAGCGCCACGGTCAGTTCGACCGTGCCCAGCCCGGAGGCGAAGTGCCCGCTGGAACGGCTCACGCTGTCGAGTAAATAGCGGCGCAGTTCGTCGCAGAGTTTCGGTAAACTCTCTTTCGGCAACAGTCGTAACTCCTGGGTGGAGTCGACCAGTGCCAGGGTCGGGTATTTGGCAATATCAAAACTCATCAGGGGCCTATTAATACTTATTGTTTATTTATTACGCTGGATGATGTAGTCCGCTAGCGCTTCCAGTGCCGAGGTATCGAGTGACTGTTCAGCCAGTTGTTTCAGCGACTGACGGGCATCGTCGATCAGATCCCGGGCTTTCTTCCGGGCTTGCTCAAGACCCAGAAGTGCAGGGTAGGTACTTTTACCAAGTTGCTGGTCGGCA</t>
+          <t>TCAGATGCTGTTCAATACCGATCAGGTTATCGAAGTGTTTGTGATTGGCGTCGGTGGCGTTGGCGGTGCGCTGCTGGAGCAACTGAAGCGTCAGCAAAGCTGGCTGAAGAATAAACATATCGACTTACGTGTCTGCGGTGTTGCCAACTCGAAGGCTCTGCTCACCAATGTACATGGCCTTAATCTGGAAAACTGGCAGGAAGAACTGGCGCAAGCCAAAGAGCCGTTTAATCTCGGGCGCTTAATTCGCCTCGTGAAAGAATATCATCTGCTGAACCCGGTCATTGTTGACTGCACTTCCAGCCAGGCAGTGGCGGATCAATATGCCGACTTCCTGCGCGAAGGTTTCCACGTTGTCACGCCGAACAAAAAGGCCAACACCTCGTCGATGGATTACTACCATCAGTTGCGTTATGCGGCGGAAAAATCGCGGCGTAAATTCCTCTATGACACCAACGTTGGGGCTGGATTACCGGTTATTGAGAACCTGCAAAATCTGCTCAATGCAGGTGATGAATTGATGAAGTTCTCCGGCATTCTTTCTGGTTCGCTTTCTTATATCTTCGGCAAGTTAGACGAAGGCATGAGTTTCTCCGAGGCGACCACGCTGGCGCGGGAAATGGGTTATACCGAACCGGACCCGCGAGATGATCTTTCTGGTATGGATGTGGCGCGTAAACTATTGATTCTCGCTCGTGAAACGGGACGTGAACTGGAGCTGGCGGATATTGAAATTGAACCTGTGCTGCCCGCAGAGTTTAACGCCGAGGGTGATGTTGCCGCTTTTATGGCGAATCTGTCACAACTCGACGATCTCTTTGCCGCGCGCGTGGCGAAGGCCCGTGATGAAGGAAAAGTTTTGCGCTATGTTGGCAATATTGATGAAGATGGCGTCTGCCGCGTGAAGATTGCCGAAGTGGATGGTAATGATCCGCTGTTCAAAGTGAAAAATGGCGAAAACGCCCTGGCCTTCTATAGCCACTATTATCAGCCGCTGCCGTTGGTACTGCGCGGATATGGTGCGGGCAATGACGTTACAGCTGCCGGTGTCTTTGCTGATCTGCTACGTACCCTCTCATGGAAGTTAGGAGTCTGACAATAGGCGTATCACGAGGCCCTTTCTACGGCCCCAAGGTCCAAACGGTGATAGGGATAACAGGGTAATGTACCATTTACGTTGACACCACCTTTCGCGTATGGCATGATAGCGCCGGGAAGAGAGTCAATTCAGGGTGGTGAATATGAATAGTTCGACAAAGATCGCATTGGTAATTACGTTACTCGATGCCATGGGGATTGGCCTTATCATGCCAGTCTTGCCAACGTTATTACGTGAATTTATTGCTTCGGAAGATATCGCTAACCACTTTGGCGTATTGCTTGCACTTTATGCGTTAATGCAGGTTATCTTTGCTCCTTGGCTTGGAAAAATGTCTGACCGATTTGGTCGGCGCCCAGTGCTGTTGTTGTCATTAATAGGCGCATCGCTGGATTACTTATTGCTGGCTTTTTCAAGTGCGCTTTGGATGCTGTATTTAGGCCGTTTGCTTTCAGGGATCACAGGAGCTACTGGGGCTGTCGCGGCATCGGTCATTGCCGATACCACCTCAGCTTCTCAACGCGTGAAGTGGTTCGGTTGGTTAGGGGCAAGTTTTGGGCTTGGTTTAATAGCGGGGCCTATTATTGGTGGTTTTGCAGGAGAGATTTCACCGCATAGTCCCTTTTTTATCGCTGCGTTGCTAAATATTGTCACTTTCCTTGTGGTTATGTTTTGGTTCCGTGAAACCAAAAATACACGTGATAATACAGATACCGAAGTAGGGGTTGAGACGCAATCAAATTCGGTGTACATCACTTTATTTAAAACGATGCCCATTTTGTTGATTATTTATTTTTCAGCGCAATTGATAGGCCAAATTCCCGCAACGGTGTGGGTGCTATTTACCGAAAATCGTTTTGGATGGAATAGCATGATGGTTGGCTTTTCATTAGCGGGTCTTGGTCTTTTACACTCAGTATTCCAAGCCTTTGTGGCAGGAAGAATAGCCACTAAATGGGGCGAAAAAACGGCAGTACTGCTCGGATTTATTGCAGATAGTAGTGCATTTGCCTTTTTAGCGTTTATATCTGAAGGTTGGTTAGTTTTCCCTGTTTTAATTTTATTGGCTGGTGGTGGGATCGCTTTACCTGCATTACAGGGAGTGATGTCTATCCAAACAAAGAGTCATCAGCAAGGTGCTTTACAGGGATTATTGGTGAGCCTTACCAATGCAACCGGTGTTATTGGCCCATTACTGTTTGCTGTTATTTATAATCATTCACTACCAATTTGGGATGGCTGGATTTGGATTATTGGTTTAGCGTTTTACTGTATTATTATCCTGCTATCAATGACCTTCATGTTGACCCCTCAAGCTCAGGGGAGTAAACAGGAGACAAGTGCTTAGTAGGGATAACAGGGTAATGATGGCGCCTCATCCCTGAAGCCAAGGCATCAAATAAAACGAAAGGCTCAGTACCCTCTCATGGAAGTTAGGAGTCTGACATGAAACTCTACAATCTGAAAGATCACAACGAGCAGGTCAGCTTTGCGCAAGCCGTAACCCAGGGGTTGGGCAAAAATCAGGGGCTGTTTTTTCCGCACGACCTGCCGGAATTCAGCCTGACTGAAATTGATGAGATGCTGAAGCTGGATTTTGTCACCCGCAGTGCGAAGATCCTCTCGGCGTTTATTGGTGATGAAATCCCACAGGAAATCCTGGAAGAGCGCGTGCGCGCGGCGTTTGCCTTCCCGGCTCCGGTCGCCAATGTTGAAAGCGATGTCGGTTGTCTGGAATTGTTCCACGGGCCAACGCTGGCATTTAAAGATTTCGGCGGTCGCTTTATGGCACAAATGCTGACCCATATTGCGGGTGATAAGCCAGTGACCATTCTGACCGCGACCTCCGGTGATACCGGAGCGGCAGTGGCTCATGCTTTCTACGGTTTACCGAATGTGAAAGTGGTTATCCTCTATCCACGAGGCAAAATCAGTCCACTGCAAGAAAAACTGTTCTGTACATTGGGCGGCAATATCGAAACTGTTGCCATCGACGGCGATTTCGATGCCTGTCAGGCGCTGGTGAAGCAGGCGTTTGATGATGAAGAACTGAAAGTGGCGCTAGGGTTAAACTCGGCTAACTCGATTAACATCAGCCGTTTGCTGGCGCAGATTTGCTACTACTTTGAAGCTGTTGCGCAGCTGCCGCAGGAGACGCGCAACCAGCTGGTTGTCTCGGTGCCAAGCGGAAACTTCGGCGATTTGACGGCGGGTCTGCTGGCGAAGTCACTCGGTCTGCCGGTGAAACGTTTTATTGCTGCGACCAACGTGAACGATACCGTGCCACGTTTCCTGCACGACGGTCAGTGGTCACCCAAAGCGACTCAGGCGACGTTATCCAACGCGATGGACGTGAGTCAGCCGAACAACTGGCCGCGTGTGGAAGAGTTGTTCCGCCGCAAAATCTGGCAACTGAAAGAGCTGGGTTATGCAGCCGTGGATGATGAAACCACGCAACAGACAATGCGTGAGTTAAAAGAACTGGGCTACACTTCGGAGCCGCACGCTGCCGTAGCTTATCGTGCGCTGCGTGATCAGTTGAATCCAGGCGAATATGGCTTGTTCCTCGGCAC</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>13.64979653795285</v>
+        <v>-28.67762991935746</v>
       </c>
       <c r="E2" t="n">
-        <v>-33.87694222802281</v>
+        <v>-11.19334412205274</v>
       </c>
       <c r="F2" t="n">
-        <v>18.98315983858089</v>
+        <v>3.326930937698307</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>AACGCGAAGGTCGGTTTTTC</t>
+          <t>TCAGATGCTGTTCAATACCGA</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>TGCCGACCAGCAACTTGG</t>
+          <t>GTGCCGAGGAACAAGCCATA</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>59.6943825309412</v>
+        <v>57.11427589555893</v>
       </c>
       <c r="J2" t="n">
-        <v>60.59430255997739</v>
+        <v>60.39246077736146</v>
       </c>
       <c r="K2" t="n">
-        <v>2315</v>
+        <v>3672</v>
       </c>
     </row>
     <row r="3">
@@ -1030,41 +878,41 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>tktA_573_12bp_sub</t>
+          <t>b0004</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>AACTTCTGAACCGGTAGCGATGAAAATCAGTTCCGGCTGACCGGCGCAGTCTTTCAGCACATAACCACCGCGCGCGATGTTTGCCAGTTGCTCTTCAGTTCGTTCCTGCTGCGCCAGGTTCTGACGGGAGAGGATCAGTGCGGTCGGGCCGTCCTGACGCTCAACACCGTATTTCCACGCGACCGCGGATTCAACCTGGTCACACGGACGCCATGTAGACATGTTCGGGGTTACGCGCAGAGAAGCGACCTGCTCAACCGGCTGGTGAGTCGGGCCGTCTTCGCCCAGACCGATGGAGTCGTGGGTGTAAACCATCACCTGACGCTGTTTCATCAGCGCAGCCATACGTACGGCGTTACGTGCGTATTCCACGAACATCAGGAAGGTGGAGGTGTACGGCAGGAAGCCACCGTGCAGGGAGATACCGTTAGCAATCGCGGTCATACCGAACTCGCGAACACCGTAGTGGATGTAGTTACCCGCAGCATCTTCGTTGATTGCTTTAGAACCAGACCACAGGGTCAGGTTAGACGGCGCCAGGTCAGCAGAACCGCCGAGGAATTCCGGCAACAGCGGACCGAACGCTTCGATAGCATTCTGAGACGCTTTACGGCTGGCGATTTTCGCCGGATTAGCCTGCAGTTTAGCGATGAACTCTTTCGCTTTAGCGTCGAAGTCAGACGGCATTTCGCCTTTCATACGGCGGGTAAATTCAGCGGCTTCCTGCGGATAAGCTTTCGCGTAAGCAGCGAATTTCTCGTTCCATGCGGATTCTTTCGCCTGGCCTGCTTCTTTCGCATCCCACTGAGCATAGATTTCAGACGGGATTTCGAACGGCGCATATTTCCAGCCCAGTTGTTCGCGGGTCAGGGCAATTTCAGCGTCGCCCAGCGGCGCACCGTGGGAGTCGTGGGTACCGGCTTTGTTCGGGGAACCGAAACCGATGATGGTTTTGCACATCAGCAGGGAAGGTTTGTCAGTCACTGCGCGCGCTTCTTCTACTGCGCGTTTGATAGATGCCGCGTCATGACCGTCGATGTCGCGAATAACGTGCCAGCCGTAAGCTTCGAAACGCATTGCGGTGTCGTCGGTGAACCAGGTGTCGTCGGTGAACCATCCCTCGACATGACCATCGATAGAAATACCGTTGTCATCGTAGAATGCAATCAGTTTACCCAGCTTCAGCGTACCCGCCAGAGAGCAAACTTCGTGGGAGATGCCTTCCATCATGCAGCCGTCGCCCATGAAGGCGTAGGTGTAGTGGTCGACAATGTCGTGGCCCGGACGGTTAAACTGCGCCGCCAGCGTTTTTTCTGCAATCGCCATACCGACTGCGTTGGCAATACCCTGACCCAGCGGACCGGTGGTGGTTTCCACACCAGCGGTGTAACCCACTTCCGGGTGACCCGGAGTTTTAGAGTGCAGCTGACGGAAGTTTTTCAGTTCTTCCATCGGCAGATCGTAACCGGTGAGGTGCAGCAGGCTGTAGATCAGCATGGAGCCGTGGCCGTTGGACAGCACGAAGCGGTCACGGTCAGCCCAGGACGGATTCTGCGGGTTGTGTTTCAGGAAATCACGCCACAGGACTTCGGCAATGTCAGCCATACCCATAGGGGCACCCGGGTGACCGGATTTGGCTTTCTGTACTGCGTCCATGCTCAGCGCACGAATAGCATTGGCAAGCTCTTTACGTGAGGACATTTTGACTCCAGATCGGATGATGAAGGGCACGCCCTTAACGACTTGACGACAGCGCGTTTTGGGCTACGCCGGAAAATTTGCCAACAATTTACCGCAAGCCGCGCGTCATGTACATGGAACATCCTTTTGCCGCTTCAGAAATCTCTGGATCATGCTCGCATGTTGCGCAATCTACTCGCCCGTCCGCTGCGCTTTTCCTTATACTGAGACTGAGCGTCGATTCACCTGCAAACGGCGCATTTTTAGAATAATCCTGACCTTGTGCGGAAGAGAAAACATGAAAATTCGCGCCTTATTGGTAGCAATGAGCGTGGCAACGGTACTGACTGGTTGCCAGAATATGGACTCCAACGGACTGCTCTCATCAGGAGCGGAAGCTTTTCAGGCTTACAGTTTGAGTGATGCGCAGGTGAAAACCCTGAGCGATCAGGCATGTCAGGAGATGGACAGCAAGGCGACGATTGCGCCAGCCAATAGCGAATACGCTAAACGTCTGACAACTATTGCCAATGCGCT</t>
+          <t>GCGTGAAGATTGCCGAAGTGGATGGTAATGATCCGCTGTTCAAAGTGAAAAATGGCGAAAACGCCCTGGCCTTCTATAGCCACTATTATCAGCCGCTGCCGTTGGTACTGCGCGGATATGGTGCGGGCAATGACGTTACAGCTGCCGGTGTCTTTGCTGATCTGCTACGTACCCTCTCATGGAAGTTAGGAGTCTGACATGGTTAAAGTTTATGCCCCGGCTTCCAGTGCCAATATGAGCGTCGGGTTTGATGTGCTCGGGGCGGCGGTGACACCTGTTGATGGTGCATTGCTCGGAGATGTAGTCACGGTTGAGGCGGCAGAGACATTCAGTCTCAACAACCTCGGACGCTTTGCCGATAAGCTGCCGTCAGAACCACGGGAAAATATCGTTTATCAGTGCTGGGAGCGTTTTTGCCAGGAACTGGGTAAGCAAATTCCAGTGGCGATGACCCTGGAAAAGAATATGCCGATCGGTTCGGGCTTAGGCTCCAGTGCCTGTTCGGTGGTCGCGGCGCTGATGGCGATGAATGAACACTGCGGCAAGCCGCTTAATGACACTCGTTTGCTGGCTTTGATGGGCGAGCTGGAAGGCCGTATCTCCGGCAGCATTCATTACGACAACGTGGCACCGTGTTTTCTCGGTGGTATGCAGTTGATGATCGAAGAAAACGACATCATCAGCCAGCAAGTGCCAGGGTTTGATGAGTGGCTGTGGGTGCTGGCGTATCCGGGGATTAAAGTCTCGACGGCAGAAGCCAGGGCTATTTTACCGGCGCAGTATCGCCGCCAGGATTGCATTGCGCACGGGCGACATCTGGCAGGCTTCATTCACGCCTGCTATTCCCGTCAGCCTGAGCTTGCCGCGAAGCTGATGAAAGATGTTATCGCTGAACCCTACCGTGAACGGTTACTGCCAGGCTTCCGGCAGGCGCGGCAGGCGGTCGCGGAAATCGGCGCGGTAGCGAGCGGTATCTCCGGCTCCGGCCCGACCTTGTTCGCTCTGTGTGACAAGCCGGAAACCGCCCAGCGCGTTGCCGACTGGTTGGGTAAGAACTACCTGCAAAATCAGGAAGGTTTTGTTCATATTTGCCGGCTGGATACGGCGGGCGCACGAGTACTGGAAAACTAAAATAGGCGTATCACGAGGCCCTTTCTACGGCCCCAAGGTCCAAACGGTGATAGGGATAACAGGGTAATGTACCATTTACGTTGACACCACCTTTCGCGTATGGCATGATAGCGCCGGGAAGAGAGTCAATTCAGGGTGGTGAATATGAATAGTTCGACAAAGATCGCATTGGTAATTACGTTACTCGATGCCATGGGGATTGGCCTTATCATGCCAGTCTTGCCAACGTTATTACGTGAATTTATTGCTTCGGAAGATATCGCTAACCACTTTGGCGTATTGCTTGCACTTTATGCGTTAATGCAGGTTATCTTTGCTCCTTGGCTTGGAAAAATGTCTGACCGATTTGGTCGGCGCCCAGTGCTGTTGTTGTCATTAATAGGCGCATCGCTGGATTACTTATTGCTGGCTTTTTCAAGTGCGCTTTGGATGCTGTATTTAGGCCGTTTGCTTTCAGGGATCACAGGAGCTACTGGGGCTGTCGCGGCATCGGTCATTGCCGATACCACCTCAGCTTCTCAACGCGTGAAGTGGTTCGGTTGGTTAGGGGCAAGTTTTGGGCTTGGTTTAATAGCGGGGCCTATTATTGGTGGTTTTGCAGGAGAGATTTCACCGCATAGTCCCTTTTTTATCGCTGCGTTGCTAAATATTGTCACTTTCCTTGTGGTTATGTTTTGGTTCCGTGAAACCAAAAATACACGTGATAATACAGATACCGAAGTAGGGGTTGAGACGCAATCAAATTCGGTGTACATCACTTTATTTAAAACGATGCCCATTTTGTTGATTATTTATTTTTCAGCGCAATTGATAGGCCAAATTCCCGCAACGGTGTGGGTGCTATTTACCGAAAATCGTTTTGGATGGAATAGCATGATGGTTGGCTTTTCATTAGCGGGTCTTGGTCTTTTACACTCAGTATTCCAAGCCTTTGTGGCAGGAAGAATAGCCACTAAATGGGGCGAAAAAACGGCAGTACTGCTCGGATTTATTGCAGATAGTAGTGCATTTGCCTTTTTAGCGTTTATATCTGAAGGTTGGTTAGTTTTCCCTGTTTTAATTTTATTGGCTGGTGGTGGGATCGCTTTACCTGCATTACAGGGAGTGATGTCTATCCAAACAAAGAGTCATCAGCAAGGTGCTTTACAGGGATTATTGGTGAGCCTTACCAATGCAACCGGTGTTATTGGCCCATTACTGTTTGCTGTTATTTATAATCATTCACTACCAATTTGGGATGGCTGGATTTGGATTATTGGTTTAGCGTTTTACTGTATTATTATCCTGCTATCAATGACCTTCATGTTGACCCCTCAAGCTCAGGGGAGTAAACAGGAGACAAGTGCTTAGTAGGGATAACAGGGTAATGATGGCGCCTCATCCCTGAAGCCAAGGCATCAAATAAAACGAAAGGCTCAACGGCGGGCGCACGAGTACTGGAAAACTAAAATCTATTCATTATCTCAATCAGGCCGGGTTTGCTTTTATGCAGCCCGGCTTTTTTATGAAGAAATTATGGAGAAAAATGACAGGGAAAAAGGAGAAATTCTCAATAAATGCGGTAACTTAGAGATTAGGATTGCGGAGAATAACAACCGCCGTTCTCATCGAGTAATCTCCGGATATCGACCCATAACGGGCAATGATAAAAGGAGTAACCTGTGAAAAAGATGCAATCTATCGTACTCGCACTTTCCCTGGTTCTGGTCGCTCCCATGGCAGCACAGGCTGCGGAAATTACGTTAGTCCCGTCAGTAAAATTACAGATAGGCGATCGTGATAATCGTGGCTATTACTGGGATGGAGGTCACTGGCGCGACCACGGCTGGTGGAAACAACATTATGAATGGCGAGGCAATCGCTGGCACCTACACGGACCGCCGCCACCGCCGCGCCACCATAAGAAAGCTCCTCATGATCATCACGGCGGTCATGGTCCAGGCAAACATCACCGCTAAATGACAAATGCCGGGTAACAATCCGGCATTCAGCGCCTGATGCGACGCTGGCGCGTCTTATCAGGCCTACGTTAATTCTGCAATATATTGAATCTGCATGCTTTTGTAGGCAGGATAAGGCGTTCACGCCGCATCCGGCATTGACTGCAAACTTAACGCTGCTCGTAGCGTTTAAACACCAGTTCGCCATTGCTGGAGGAATCTTCATCAAAGAAGTAACCTTCGCTATTAAAACCAGTCAGTTGCTCTGGTTTGGTCAGCCGATTTTCAATAATGAAACGACTCATCAGACCGCGTGCTTTCTTAGCGTAGAAGCTGATGATCTTAAATTTGCCGTTCTTCTCATCGAGGAACACCGGCTTGATAATCTCGGCATTCAATTTCTTCGGCTTCACCGATTTAAAATACTCATCTGACGCCAGATTAATCACCACATTATCGCCTTGTGCTGCGAGCGCCTCGTTCAGCTTGTTGGTGATGATATCTCCCCAGAATTGATACAGATCTTTCCCTCGGGCATTCTCAAGACGGATCCCCATTTCCAGACGATAAGGCTGCATTAAATCGAGCGGGCGGAGTACGCCATACAAGCCGGAAAGCATTCGCAAATGCTGTTGGGCAAAATCGAAATCGTCTTCGCTGAAGGTTTCG</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>14.25874858550679</v>
+        <v>-46.32795461786364</v>
       </c>
       <c r="E3" t="n">
-        <v>9.051540840486894</v>
+        <v>12.95336201406417</v>
       </c>
       <c r="F3" t="n">
-        <v>-8.990713976036261</v>
+        <v>4.833942337509598</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>AACTTCTGAACCGGTAGCGA</t>
+          <t>GCGTGAAGATTGCCGAAGTG</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>AGCGCATTGGCAATAGTTGTC</t>
+          <t>CGAAACCTTCAGCGAAGACG</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>59.03603785987434</v>
+        <v>60.17921481643259</v>
       </c>
       <c r="J3" t="n">
-        <v>59.86697546596565</v>
+        <v>59.56499199245616</v>
       </c>
       <c r="K3" t="n">
-        <v>2217</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="4">
@@ -1073,127 +921,41 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>aceE_del</t>
+          <t>b0005</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ACGTAAAGTCTACATTTGTGCATAGTTACAACTTTGAAACGTTATATATGTCAAGTTGTTAAAATGTGCACAGTTTCATGATTTCAATCAAAACCTGTATGGACATAAGGTGAATACTTTGTTACTTTAGCGTCACAGACATGAAATTGGTAAGACCAATTGACTTCGGCAAGTGGCTTAAGACAGGAACTCATGGCCTACAGCAAAATCCGCCAACCAAAACTCTCCGATGTGATTGAGCAGCAACTGGAGTTTTTGATCCTCGAAGGCACTCTCCGCCCGGGCGAAAAACTCCCACCGGAACGCGAACTGGCAAAACAGTTTGACGTCTCCCGTCCCTCCTTGCGTGAGGCGATTCAACGTCTCGAAGCGAAGGGCTTGTTGCTTCGTCGCCAGGGTGGCGGCACTTTTGTCCAGAGCAGCCTATGGCAAAGCTTCAGCGATCCGCTGGTGGAGCTGCTCTCCGACCATCCTGAGTCACAGTATGACTTGCTCGAAACACGACACGCCCTGGAAGGTATCGCCGCTTATTACGCCGCGCTGCGTAGTACCGATGAAGACAAGGAACGCATCCGTGAACTCCACCACGCCATAGAGCTGGCGCAGCAGTCTGGCGATCTGGACGCGGAATCAAACGCCGTACTCCAGTATCAGATTGCCGTCACCGAAGCGGCCCACAATGTGGTTCTGCTTCATCTGCTAAGGTGTATGGAGCCGATGTTGGCCCAGAATGTCCGCCAGAACTTCGAATTGCTCTATTCGCGTCGCGAGATGCTGCCGCTGGTGAGTAGTCACCGCACCCGCATATTTGAAGCGATTATGGCCGGTAAGCCGGAAGAAGCGCGCGAAGCATCGCATCGCCATCTGGCCTTTATCGAAGAAATTTTGCTCGACAGAAGTCGTGAAGAGAGCCGCCGTGAGCGTTCTCTGCGTCGTCTGGAGCAACGAAAGAATTAGTGATTTTTCTGGTAAAAATTATCCAGAAGATGTTGTAAATCAAGCGCATATAAAAGCGCGGCAACTAAACGTAGAACCTGTCTTATTGAGCTTTCCGGCGAGAGTTCAATGGGACAGGTTCCAGAAAACTCAACGTTATTAGATAGATAAGGAATAACCCAATAGGCGTATCACGAGGCCCTTTCTACGGCCCCAAGGTCCAAACGGTGATAGGGATAACAGGGTAATGTACCATTTACGTTGACACCACCTTTCGCGTATGGCATGATAGCGCCGGGAAGAGAGTCAATTCAGGGTGGTGAATATGAATAGTTCGACAAAGATCGCATTGGTAATTACGTTACTCGATGCCATGGGGATTGGCCTTATCATGCCAGTCTTGCCAACGTTATTACGTGAATTTATTGCTTCGGAAGATATCGCTAACCACTTTGGCGTATTGCTTGCACTTTATGCGTTAATGCAGGTTATCTTTGCTCCTTGGCTTGGAAAAATGTCTGACCGATTTGGTCGGCGCCCAGTGCTGTTGTTGTCATTAATAGGCGCATCGCTGGATTACTTATTGCTGGCTTTTTCAAGTGCGCTTTGGATGCTGTATTTAGGCCGTTTGCTTTCAGGGATCACAGGAGCTACTGGGGCTGTCGCGGCATCGGTCATTGCCGATACCACCTCAGCTTCTCAACGCGTGAAGTGGTTCGGTTGGTTAGGGGCAAGTTTTGGGCTTGGTTTAATAGCGGGGCCTATTATTGGTGGTTTTGCAGGAGAGATTTCACCGCATAGTCCCTTTTTTATCGCTGCGTTGCTAAATATTGTCACTTTCCTTGTGGTTATGTTTTGGTTCCGTGAAACCAAAAATACACGTGATAATACAGATACCGAAGTAGGGGTTGAGACGCAATCAAATTCGGTGTACATCACTTTATTTAAAACGATGCCCATTTTGTTGATTATTTATTTTTCAGCGCAATTGATAGGCCAAATTCCCGCAACGGTGTGGGTGCTATTTACCGAAAATCGTTTTGGATGGAATAGCATGATGGTTGGCTTTTCATTAGCGGGTCTTGGTCTTTTACACTCAGTATTCCAAGCCTTTGTGGCAGGAAGAATAGCCACTAAATGGGGCGAAAAAACGGCAGTACTGCTCGGATTTATTGCAGATAGTAGTGCATTTGCCTTTTTAGCGTTTATATCTGAAGGTTGGTTAGTTTTCCCTGTTTTAATTTTATTGGCTGGTGGTGGGATCGCTTTACCTGCATTACAGGGAGTGATGTCTATCCAAACAAAGAGTCATCAGCAAGGTGCTTTACAGGGATTATTGGTGAGCCTTACCAATGCAACCGGTGTTATTGGCCCATTACTGTTTGCTGTTATTTATAATCATTCACTACCAATTTGGGATGGCTGGATTTGGATTATTGGTTTAGCGTTTTACTGTATTATTATCCTGCTATCAATGACCTTCATGTTGACCCCTCAAGCTCAGGGGAGTAAACAGGAGACAAGTGCTTAGTAGGGATAACAGGGTAATGATGGCGCCTCATCCCTGAAGCCAAGGCATCAAATAAAACGAAAGGCTCACAACGTTATTAGATAGATAAGGAATAACCCGAGGTAAAAGAATAATGGCTATCGAAATCAAAGTACCGGACATCGGGGCTGATGAAGTTGAAATCACCGAGATCCTGGTCAAAGTGGGCGACAAAGTTGAAGCCGAACAGTCGCTGATCACCGTAGAAGGCGACAAAGCCTCTATGGAAGTTCCGTCTCCGCAGGCGGGTATCGTTAAAGAGATCAAAGTCTCTGTTGGCGATAAAACCCAGACCGGCGCACTGATTATGATTTTCGATTCCGCCGACGGTGCAGCAGACGCTGCACCTGCTCAGGCAGAAGAGAAGAAAGAAGCAGCTCCGGCAGCAGCACCAGCGGCTGCGGCGGCAAAAGACGTTAACGTTCCGGATATCGGCAGCGACGAAGTTGAAGTGACCGAAATCCTGGTGAAAGTTGGCGATAAAGTTGAAGCTGAACAGTCGCTGATCACCGTAGAAGGCGACAAGGCTTCTATGGAAGTTCCGGCTCCGTTTGCTGGCACCGTGAAAGAGATCAAAGTGAACGTGGGTGACAAAGTGTCTACCGGCTCGCTGATTATGGTCTTCGAAGTCGCGGGTGAAGCAGGCGCGGCAGCTCCGGCCGCTAAACAGGAAGCAGCTCCGGCAGCGGCCCCTGCACCAGCGGCTGGCGTGAAAGAAGTTAACGTTCCGGATATCGGCGGTGACGAAGTTGAAGTGACTGAAGTGATGGTGAAAGTGGGCGACAAAGTTGCCGCTGAACAGTCACTGATCACCGTAGAAGGCGACAAAGCTTCTATGGAAGTTCCGGCGCCGTTTGCAGGCGTCGTGAAGGAACTGAAAGTCAACGTTGGCGATAAAGTGAAAACTGGCTCGCTGATTATGATCTTCGAAGTTGAAGGCGCAGCGCCTGCGGCAGCTCCTGCGAAACAGGAAGCGGCAGCGCCGGCACCGGCAGCAAAAGCTGAAGCCCCGGCAGCAGCACCAGCTGCGAAAGCGGAAGGCAAATCTGAATTTGCTGAAAACGACGCTTATGTTCACGCGACTCCGCTGATCCGCCGTCTGGCACGCGAGTTTGGTGTTAACCTTGCGAAAGTGAAGGGCACTGGCCGTAAAGGTCGTATCCTGCGCGAAGACGTTCAGGCTTACGTGAAAGAAGCTATCAAACGTGCAGAAGCAGCTCC</t>
+          <t>TGACCATTCTGACCGCGACCTCCGGTGATACCGGAGCGGCAGTGGCTCATGCTTTCTACGGTTTACCGAATGTGAAAGTGGTTATCCTCTATCCACGAGGCAAAATCAGTCCACTGCAAGAAAAACTGTTCTGTACATTGGGCGGCAATATCGAAACTGTTGCCATCGACGGCGATTTCGATGCCTGTCAGGCGCTGGTGAAGCAGGCGTTTGATGATGAAGAACTGAAAGTGGCGCTAGGGTTAAACTCGGCTAACTCGATTAACATCAGCCGTTTGCTGGCGCAGATTTGCTACTACTTTGAAGCTGTTGCGCAGCTGCCGCAGGAGACGCGCAACCAGCTGGTTGTCTCGGTGCCAAGCGGAAACTTCGGCGATTTGACGGCGGGTCTGCTGGCGAAGTCACTCGGTCTGCCGGTGAAACGTTTTATTGCTGCGACCAACGTGAACGATACCGTGCCACGTTTCCTGCACGACGGTCAGTGGTCACCCAAAGCGACTCAGGCGACGTTATCCAACGCGATGGACGTGAGTCAGCCGAACAACTGGCCGCGTGTGGAAGAGTTGTTCCGCCGCAAAATCTGGCAACTGAAAGAGCTGGGTTATGCAGCCGTGGATGATGAAACCACGCAACAGACAATGCGTGAGTTAAAAGAACTGGGCTACACTTCGGAGCCGCACGCTGCCGTAGCTTATCGTGCGCTGCGTGATCAGTTGAATCCAGGCGAATATGGCTTGTTCCTCGGCACCGCGCATCCGGCGAAATTTAAAGAGAGCGTGGAAGCGATTCTCGGTGAAACGTTGGATCTGCCAAAAGAGCTGGCAGAACGTGCTGATTTACCCTTGCTTTCACATAATCTGCCCGCCGATTTTGCTGCGTTGCGTAAATTGATGATGAATCATCAGTAAAATCTATTCATTATCTCAATCAGGCCGGGTTTGCTTTTATGCAGCCCGGCTTTTTTATGAAGAAATTATGGAGAAAAATGACAGGGAAAAAGGAGAAATTCTCAATAAATGCGGTAACTTAGAGATTAGGATTGCGGAGAATAACAACCGCCGTTCTCATCGAGTAATCTCCGGATATCGACCCATAACGGGCAATGATAAAAGGAGTAACCTAATAGGCGTATCACGAGGCCCTTTCTACGGCCCCAAGGTCCAAACGGTGATAGGGATAACAGGGTAATGTACCATTTACGTTGACACCACCTTTCGCGTATGGCATGATAGCGCCGGGAAGAGAGTCAATTCAGGGTGGTGAATATGAATAGTTCGACAAAGATCGCATTGGTAATTACGTTACTCGATGCCATGGGGATTGGCCTTATCATGCCAGTCTTGCCAACGTTATTACGTGAATTTATTGCTTCGGAAGATATCGCTAACCACTTTGGCGTATTGCTTGCACTTTATGCGTTAATGCAGGTTATCTTTGCTCCTTGGCTTGGAAAAATGTCTGACCGATTTGGTCGGCGCCCAGTGCTGTTGTTGTCATTAATAGGCGCATCGCTGGATTACTTATTGCTGGCTTTTTCAAGTGCGCTTTGGATGCTGTATTTAGGCCGTTTGCTTTCAGGGATCACAGGAGCTACTGGGGCTGTCGCGGCATCGGTCATTGCCGATACCACCTCAGCTTCTCAACGCGTGAAGTGGTTCGGTTGGTTAGGGGCAAGTTTTGGGCTTGGTTTAATAGCGGGGCCTATTATTGGTGGTTTTGCAGGAGAGATTTCACCGCATAGTCCCTTTTTTATCGCTGCGTTGCTAAATATTGTCACTTTCCTTGTGGTTATGTTTTGGTTCCGTGAAACCAAAAATACACGTGATAATACAGATACCGAAGTAGGGGTTGAGACGCAATCAAATTCGGTGTACATCACTTTATTTAAAACGATGCCCATTTTGTTGATTATTTATTTTTCAGCGCAATTGATAGGCCAAATTCCCGCAACGGTGTGGGTGCTATTTACCGAAAATCGTTTTGGATGGAATAGCATGATGGTTGGCTTTTCATTAGCGGGTCTTGGTCTTTTACACTCAGTATTCCAAGCCTTTGTGGCAGGAAGAATAGCCACTAAATGGGGCGAAAAAACGGCAGTACTGCTCGGATTTATTGCAGATAGTAGTGCATTTGCCTTTTTAGCGTTTATATCTGAAGGTTGGTTAGTTTTCCCTGTTTTAATTTTATTGGCTGGTGGTGGGATCGCTTTACCTGCATTACAGGGAGTGATGTCTATCCAAACAAAGAGTCATCAGCAAGGTGCTTTACAGGGATTATTGGTGAGCCTTACCAATGCAACCGGTGTTATTGGCCCATTACTGTTTGCTGTTATTTATAATCATTCACTACCAATTTGGGATGGCTGGATTTGGATTATTGGTTTAGCGTTTTACTGTATTATTATCCTGCTATCAATGACCTTCATGTTGACCCCTCAAGCTCAGGGGAGTAAACAGGAGACAAGTGCTTAGTAGGGATAACAGGGTAATGATGGCGCCTCATCCCTGAAGCCAAGGCATCAAATAAAACGAAAGGCTCACATAACGGGCAATGATAAAAGGAGTAACCTATGACAAATGCCGGGTAACAATCCGGCATTCAGCGCCTGATGCGACGCTGGCGCGTCTTATCAGGCCTACGTTAATTCTGCAATATATTGAATCTGCATGCTTTTGTAGGCAGGATAAGGCGTTCACGCCGCATCCGGCATTGACTGCAAACTTAACGCTGCTCGTAGCGTTTAAACACCAGTTCGCCATTGCTGGAGGAATCTTCATCAAAGAAGTAACCTTCGCTATTAAAACCAGTCAGTTGCTCTGGTTTGGTCAGCCGATTTTCAATAATGAAACGACTCATCAGACCGCGTGCTTTCTTAGCGTAGAAGCTGATGATCTTAAATTTGCCGTTCTTCTCATCGAGGAACACCGGCTTGATAATCTCGGCATTCAATTTCTTCGGCTTCACCGATTTAAAATACTCATCTGACGCCAGATTAATCACCACATTATCGCCTTGTGCTGCGAGCGCCTCGTTCAGCTTGTTGGTGATGATATCTCCCCAGAATTGATACAGATCTTTCCCTCGGGCATTCTCAAGACGGATCCCCATTTCCAGACGATAAGGCTGCATTAAATCGAGCGGGCGGAGTACGCCATACAAGCCGGAAAGCATTCGCAAATGCTGTTGGGCAAAATCGAAATCGTCTTCGCTGAAGGTTTCGGCCTGCAAGCCGGTGTAGACATCACCTTTAAACGCCAGAATCGCCTGGCGGGCATTCGCCGGCGTGAAATCTGGCTGCCAGTCATGAAAGCGAGCGGCGTTGATACCCGCCAGTTTGTCGCTGATGCGCATCAGCGTGCTAATCTGCGGAGGCGTCAGTTTCCGCGCCTCATGGATCAACTGCTGGGAATTGTCTAACAGCTCCGGCAGCGTATAGCGCGTGGTGGTCAACGGGCTTTGGTAATCAAGCGTTTTCGCAGGTGAAATAAGAATCAGCATATCCAGTCCTTGCAGGAAATTTATGCCGACTTTAGCAAAAAATGAGAATGAGTTGATCGATAGTTGTGATTACTCCTGCGAAACATCATCCCACGCGTCCGGAGAAAGCTGGCGACCGATATCCGGATAACGCAATGGATCAAACACCGGGCGCACGCCGAGTTTACGCTGGCGTAGATAATCACTGGCAATGGTATGAACCACAGGCGAGAGCAGTAAAATGGCG</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>-42.60669801557233</v>
+        <v>5.885215896573129</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.900577242230667</v>
+        <v>-34.68241902366907</v>
       </c>
       <c r="F4" t="n">
-        <v>-6.517879085020752</v>
+        <v>-29.54156409016912</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>ACGTAAAGTCTACATTTGTGCA</t>
+          <t>TGACCATTCTGACCGCGAC</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>GGAGCTGCTTCTGCACGTTT</t>
+          <t>CGCCATTTTACTGCTCTCGC</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>56.32043528895827</v>
+        <v>60.08009301751491</v>
       </c>
       <c r="J4" t="n">
-        <v>61.51048014864102</v>
+        <v>59.97319661701511</v>
       </c>
       <c r="K4" t="n">
-        <v>3706</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>pntA_promoter_sub</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>TAATTTCGCCCGCACGGATCACGGTCACGCCGCGAATCACCACATCATCAAAATCAACAGTGATATTGCCGTCTTTCTCTTTGCACAACAGTTTCAGCAGATTAACGAGGTTTGTGCCGTAAAGCTGTGAGGATTGCGTCGGCAGACGGCCCGGAAGATCGGTATAACCAATCACTTTGACACCATTTTCCGTAGTGAAGATTTCACCCGGCACGGTGTATTCACAGTTGCCGCCGTTTTGGGCTGCCAGGTCGACAATCACACTGCCCGCCTTCATGGAGTCAACCATTTCACGGGTAATTAGCTTCGGCGCTGGTTTGCCTGGAATAAGCGCGGTGGTGACAATGATATCGACCTCTTTTGCCTGGGCGGCAAAGAGTTCCATTTCCGCTTTGATGAACGCGTCCGACATCACTTTGGCATAGCCATCGCCGCTGCCAGCTTCCTCTTTAAAATCCAGCTCGAGGAATTCCGCGCCCATACTTTGAACTTGTTCTTTCACTTCCGGGCGGGTGTCGAATGCACGCACAATCGCGCCGAGACTGTTTGCTGCGCCAATGGCGGCCAGACCTGCAACACCCGCACCAATCACCATCACTTTTGCCGGTGGCACTTTCCCGGCCGCAGTAATTTGCCCGGTAAAGAAGCGCCCAAATTCATGTGCCGCTTCAACAATGGCGCGATAACCGGCGATGTTCGCCATCGAGCTTAGTGCGTCCAGCGATTGTGCGCGTGAGATACGCGGCACAGAGTCCATCGCCATCACGGTCACGTTACGTTCCGCAAGTTTTTGCATTAATTCCGGATTCTGCGCAGGCCAGATAAAACTCACCAGCGTTGTCCCAGGATTCAGTAACGCAATTTCATCATCTAACGGCGCATTGACCTTCAGAATGATCTCTGACTGCCAGACGCTATTCCCTTCTACAATTTCAGCGCCCGCTTGCACAAACGCTTTATCGTCAAAACTTGCCAGTTGACCCGCGCCGCTCTCTACCGCGACGGTAAAACCCAGTTTCAGCAGCTGTTCCACTGTTTTTGGCGTTGCTGCAACACGGGTTTCATTGGTTAACCGTTCTCTTGGTATGCCAATTCGCATCTAGATTCGTGCTAGCATTATACCTAGGACTGAGCTAGCTGTCAAGGCGCGGTGATAGTGGGATAAACACCTTAGAACGCCGGATAAAGACTGATAATTGTCTTCGACGGTCGGGTAAAACGAGACATCGCCCCGGCACGAATCACTACTTAACATTAAATTAACTTATACAATTCAGTTGCTTCAGTAGTAATGATGCTGATACGGCTGTTTTTTAAGCATAGACGGTCATTTGAGCAGGATTAAAATTGGCTTAAGGAATGTGATATGAAAAATGACGCAGACAGTTACACCGTTTAAATGCAATAATCAGCCACGTTTCTCGTTAATAACAATACCAGTACCTGGTTTGCGCAAGGCGAAGGATTATTTTTATGAAGCTTAAGAACACCCTCCTGGCGTCGGCACTGCTTTCTGCTATGGCATTCTCCGTTAACGCAGCAACAGAACTGACACCGGAGCAAGCGGCAGCGGTTAAACCTTTTGACCGTGTAGTGGTTACCGGTCGTTTTAATGCTATTGGCGAAGCGGTGAAAGCCGTTTCTCGTCGCGCAGATAAAGAAGGTGCCGCCTCTTTTTATGTTGTCGACACTTCTGATTTTGGTAACAGCGGTAACTGGCGTGTGGTCGCTGACCTCTATAAAGCCGATGCTGAAAAAGCAGAAGAAACAAGTAATCGCGTAATTAACGGTGTTGTCGAACTGCCGAAAGATCAGGCTGTTCTGATTGAACCGTTTGACACGGTCACCGTCCAGGGCTTCTATCGTAGCCAGCCAGAAGTCAATGATGCCATCACCAAAGCGGCAAAAGCGAAAGGTGCCTACTCTTTCTACATCGTTCGTCAAATCGATGCCAACCAGGGCGGCAACCAGCGTATTACTGCATTCATCTATAAAAAAGATGCTAAGAAACGTATCGTCCAGAGCCCGGATGTGATCCCGGCAGATTCCGAAGCAGGACGTGCAGCTCTGGCTGCCGGTGGCGAAGCCGCGAAGAAAGTTGAGATCCCGGGTGTTGCGACTACCGCATCACCAAGTTCTGAAGTCGGTCGCTTCTTTGAAACCCAGTCATCAAAAGGCGGGCGTTACACCGTCACGCTCCCGGATGGCACTAAAGTCGAAGAACTGAACAAAGCGACCGCAGCGATGATGGTCCCGTTCGACA</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>8.32323228564394</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-14.63116813722309</v>
-      </c>
-      <c r="F5" t="n">
-        <v>10.99409519360194</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>TAATTTCGCCCGCACGGAT</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>TGTCGAACGGGACCATCATC</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>60.15332929800883</v>
-      </c>
-      <c r="J5" t="n">
-        <v>59.82515507935778</v>
-      </c>
-      <c r="K5" t="n">
-        <v>2263</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Cgl1452_ins</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>AGTCGCTAAAGTCAGGCCATCTTTTTCAACAGGTGATGGATCGCCATGACAAACTTCACGACCAGCACGCCGCATGATGCATTATTTAAAACCTTTCTCACGCACCCTGACACTGCGCGGGATTTTATGGAGATTCACTTACCTAAAGATTTACGTGAACTGTGCGATCTCGATAGCTTAAAACTGGAATCCGCCAGCTTTGTCGATGAAAAATTGCGGGCGCTACACTCCGATATTTTATGGTCGGTAAAGACCCGCGAAGGCGATGGCTATATCTATGTGGTGATTGAACATCAGAGCCGCGAGGACATTCATATGGCCTTTCGCCTGATGCGCTATTCCATGGCGGTGATGTAGCGCCATATAGAGCATGATAAACGCCAGCCGCTACCGTTGGTCATCCCGATGCTATTTTATCACGGTAGCCGTAGTCCTTACCCCTGGTCCCTGTGCTGGCTGGACGAATTTGCCGACCCGACTACCGCACGGAAGCTTTATAACGCCGCGTTCCCGCTGGTGGATGTTACTGTCGTGCCAGACGACGAGATTGTGCAGCATCGCAGAGTCGCCCTGTTGGAGTTGATCCAAAAGCATATTCGCCAGCGCGATCTGATGGGGCTTATCGATCAACTGGTAGTATTACTGGTTACAGAGTGTGCTAATGACAGCCAGATAACTGCGCTGTTAAATTACATTTTACTGACTGGCGATGAAGCGCGTTTTAATGAGTTTATCAGTGAACTTACCCGTCGAATGCCACAACACAGGGAGCGAATAATGACGATTGCAGAGCGAATTCATAATGATGGATATATAAAAGGGGAGCAGCGCATTCTTCGATTGTTGTTGCAGAATGGGGCGGATCCTGAATGGATACAAAAGATTACCGGACTTTCGGCAGAGCAAATGCAGGCATTAAGGCAGCCCTTGCCTGAGCGTGAGCGCTATTCATGGCTCAAGAGCTAATCAGAGACGGATGACAAACGCAAAGCAGCCTGATGCGCTATGCTTATCAGGTCTACATAACCCATTAAATATATTGAACTTTAAAGATTTTTGTAGACCTGGTCAGGCGTTCACATGTCCGGCGACCGCTCCGAGGTTGAAGCTTAAGCATCCGGCATGAACAAAGCGTACTTTGCTTAATTCAGGCTGGAACGTGGCGATGACCCAGCAAAGATAAAACGAGTCACAGGTTATGCATGAGAGGAAATCAGGCGCTTCGCCGCTATTTCGAATTTATTCCATTGCCCGATACACGGCCTCGCCAATTTGCTTCAGTGCTTCGCGATAGGTTTCGCTGAGCGGCAAAGCGCAGTTGATGCGCAGACAATTACGGTATTTGCCGGAAGCTGAGAAAATCGAGCCTGCCGCCACCTGGATTTTCATGCGGCACAGCTGCCGCGCGACGCAGACCATATCGACCTGTTCAGGCAATTCTATCCACAGTAAAAATCCGCCTTTCGGGCGCGTAATACAGATTTCGCAGGGAAAATATTCCCGTATCCAGCAGGTATAAAGCGCCAAATTGCGCTGATAGATCTGCCGCATCCGCCGGATATGGCGATGATAGTGACCTTCCAGCACAAACGTTGCCGCCGCCATTTGCGTGGACGGCACATTAAAGCTGCTGATGGCGTATTTCATATGCATCAGTTTATCGTGATAACGCCCCGGTGCGACCCAACCCACGCGCAGGCCTGGTGCAATACTTTTACTGAACGAGCTGCACAACAGCACTCGCCCGTCGATATCCCAGGAATGAATGGTCCGCGGGCGCGGATACTCCGTCGCCAGTTCGCCATAGACATCATCTTCAAAAATCACAATATCATGACGCTGAGCGAGAGAGAGAACGGCCCGTTTGCGCGCGTCCGGCATAATAAATCCCAGCGGATTATTACAGTTTGGCACCAGAATGATGCCTTTAATCGGCCACTGTTCCAGCGCCAGTTCCAGCGCTTCAACGCTGATGCCAGTTTCTGGATCGGTTGGGATTTCAATCACTTTCACGCCCATGCCGCGCAGCATCTGCATCGAACCGTAATAACAGGGGGATTCGACCGCGACAATATCGCCCGGTTTACACACTGCCATTAACGCCAGCGACATCGAGTTATGGCAGCCGCTGGTGATGATGATGTCATCGGCGGTGACCACCGAGCCGCTGTCGAGCATCAGGCGGGCAATCTGCTCTCGCAATACTCGCTGACCGGCTAACAAGTCA</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>2.763999345539332</v>
-      </c>
-      <c r="E6" t="n">
-        <v>-0.263335569570756</v>
-      </c>
-      <c r="F6" t="n">
-        <v>2.876222107101569</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>AGTCGCTAAAGTCAGGCCAT</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>TGACTTGTTAGCCGGTCAGC</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>59.09464305682206</v>
-      </c>
-      <c r="J6" t="n">
-        <v>60.32042093038291</v>
-      </c>
-      <c r="K6" t="n">
-        <v>2227</v>
+        <v>3724</v>
       </c>
     </row>
   </sheetData>
@@ -1207,110 +969,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>PRIMER_LEFT_WHOLE_SEQUENCE</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>PRIMER_RIGHT_WHOLE_SEQUENCE</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>PRIMER_LEFT_TM</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>PRIMER_RIGHT_TM</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>PRODUCT_SEQUENCE</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>PRIMER_PRODUCT_SIZE</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>PRIMER_LEFT_TM_HOMODIMER</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>PRIMER_RIGHT_TM_HOMODIMER</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>PRIMER_PAIR_TM_HETERODIMER</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Cgl1452_ins</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CGCGCCAAAAAGAGTATTGACT</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>GGCCTCGTGATACGCCTATTTTAAGCTTCAACCTCGGAGCG</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>54.09291094564452</v>
-      </c>
-      <c r="F2" t="n">
-        <v>68.74232186058538</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>CGCGCCAAAAAGAGTATTGACTTCGCATCTTTTTGTACCCATAATTATTTCATTCACATCACACAGGAAAGGCCCATAATGCCGTCAAGTACGATCAATAACATGACTAATGGAGATAATCTCGCACAGATCGGCGTTGTAGGCCTAGCAGTAATGGGCTCAAACCTCGCCCGCAACTTCGCCCGCAACGGCAACACTGTCGCTGTCTACAACCGCAGCACTGACAAAACCGACAAGCTCATCGCCGATCACGGCTCCGAAGGCAACTTCATCCCTTCTGCAACCGTCGAAGAGTTCGTAGCATCCCTGGAAAAGCCACGCCGCGCCATCATCATGGTTCAGGCTGGTAACGCCACCGACGCAGTCATCAACCAGCTGGCAGATGCCATGGACGAAGGCGACATCATCATCGACGGCGGCAACGCCCTCTACACCGACACCATTCGTCGCGAGAAGGAAATCTCCGCACGCGGTCTCCACTTCGTCGGTGCTGGTATCTCCGGCGGCGAAGAAGGCGCACTCAACGGCCCATCCATCATGCCTGGTGGCCCAGCAAAGTCCTACGAGTCCCTCGGACCACTGCTTGAGTCCATCGCTGCCAACGTTGACGGCACCCCATGTGTCACCCACATCGGCCCAGACGGCGCCGGCCACTTCGTCAAGATGGTCCACAACGGCATCGAGTACGCCGACATGCAGGTCATCGGCGAGGCATACCACCTTCTCCGCTACGCAGCAGGCATGCAGCCAGCTGAAATCGCTGAGGTTTTCAAGGAATGGAACGCAGGCGACCTGGATTCCTACCTCATCGAAATCACCGCAGAGGTTCTCTCCCAGGTGGATGCTGAAACCGGCAAGCCACTAATCGACGTCATCGTTGACGCTGCAGGTCAGAAGGGCACCGGACGTTGGACCGTCAAGGCTGCTCTTGATCTGGGTATTGCTACCACCGGCATCGGCGAAGCTGTTTTCGCACGTGCACTCTCCGGCGCAACCAGCCAGCGCGCTGCAGCACAGGGCAACCTACCTGCAGGTGTCCTCACCGATCTGGAAGCACTTGGCGTGGACAAGGCACAGTTCGTCGAAGACGTTCGCCGTGCACTGTACGCATCCAAGCTTGTTGCTTACGCACAGGGCTTCGACGAGATCAAGGCTGGCTCCGACGAGAACAACTGGGACGTTGACCCTCGCGACCTCGCTACCATCTGGCGCGGCGGCTGCATCATTCGCGCTAAGTTCCTCAACCGCATCGTCGAAGCATACGATGCAAACGCTGAACTTGAGTCCCTGCTGCTCGATCCTTACTTCAAGAGCGAGCTCGGCGACCTCATCGATTCATGGCGTCGCGTGATTGTCACCGCCACCCAGCTTGGCCTGCCAATCCCAGTGTTCGCTTCCTCCCTGTCCTACTACGACAGCCTGCGTGCAGAGCGTCTGCCAGCAGCCCTGATCCAAGGACAGCGCGACTTCTTCGGTGCGCACACCTACAAGCGCATCGACAAGGATGGCTCCTTCCACACCGAGTGGTCCGGCGACCGCTCCGAGGTTGAAGCTTAAAATAGGCGTATCACGAGGCC</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>1577</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-2.760358960867222</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-4.023749354511722</v>
-      </c>
-      <c r="K2" t="n">
-        <v>3.164417210860279</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1321,7 +987,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1387,7 +1053,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dxs_sub_933_C_T_sub</t>
+          <t>b0003</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1430,7 +1096,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>tktA_573_12bp_sub</t>
+          <t>b0004</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1473,7 +1139,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>aceE_del</t>
+          <t>b0005</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1507,92 +1173,6 @@
         <v>58.83935928832585</v>
       </c>
       <c r="K4" t="n">
-        <v>1418</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>pntA_promoter_sub</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>AATAGGCGTATCACGAGGCCCTTTCTACGGCCCCAAGGTCCAAACGGTGATAGGGATAACAGGGTAATGTACCATTTACGTTGACACCACCTTTCGCGTATGGCATGATAGCGCCGGGAAGAGAGTCAATTCAGGGTGGTGAATATGAATAGTTCGACAAAGATCGCATTGGTAATTACGTTACTCGATGCCATGGGGATTGGCCTTATCATGCCAGTCTTGCCAACGTTATTACGTGAATTTATTGCTTCGGAAGATATCGCTAACCACTTTGGCGTATTGCTTGCACTTTATGCGTTAATGCAGGTTATCTTTGCTCCTTGGCTTGGAAAAATGTCTGACCGATTTGGTCGGCGCCCAGTGCTGTTGTTGTCATTAATAGGCGCATCGCTGGATTACTTATTGCTGGCTTTTTCAAGTGCGCTTTGGATGCTGTATTTAGGCCGTTTGCTTTCAGGGATCACAGGAGCTACTGGGGCTGTCGCGGCATCGGTCATTGCCGATACCACCTCAGCTTCTCAACGCGTGAAGTGGTTCGGTTGGTTAGGGGCAAGTTTTGGGCTTGGTTTAATAGCGGGGCCTATTATTGGTGGTTTTGCAGGAGAGATTTCACCGCATAGTCCCTTTTTTATCGCTGCGTTGCTAAATATTGTCACTTTCCTTGTGGTTATGTTTTGGTTCCGTGAAACCAAAAATACACGTGATAATACAGATACCGAAGTAGGGGTTGAGACGCAATCAAATTCGGTGTACATCACTTTATTTAAAACGATGCCCATTTTGTTGATTATTTATTTTTCAGCGCAATTGATAGGCCAAATTCCCGCAACGGTGTGGGTGCTATTTACCGAAAATCGTTTTGGATGGAATAGCATGATGGTTGGCTTTTCATTAGCGGGTCTTGGTCTTTTACACTCAGTATTCCAAGCCTTTGTGGCAGGAAGAATAGCCACTAAATGGGGCGAAAAAACGGCAGTACTGCTCGGATTTATTGCAGATAGTAGTGCATTTGCCTTTTTAGCGTTTATATCTGAAGGTTGGTTAGTTTTCCCTGTTTTAATTTTATTGGCTGGTGGTGGGATCGCTTTACCTGCATTACAGGGAGTGATGTCTATCCAAACAAAGAGTCATCAGCAAGGTGCTTTACAGGGATTATTGGTGAGCCTTACCAATGCAACCGGTGTTATTGGCCCATTACTGTTTGCTGTTATTTATAATCATTCACTACCAATTTGGGATGGCTGGATTTGGATTATTGGTTTAGCGTTTTACTGTATTATTATCCTGCTATCAATGACCTTCATGTTGACCCCTCAAGCTCAGGGGAGTAAACAGGAGACAAGTGCTTAGTAGGGATAACAGGGTAATGATGGCGCCTCATCCCTGAAGCCAAGGCATCAAATAAAACGAAAGGCTCA</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>-18.06656264433227</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-42.9625693662399</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-7.940638660056891</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>AATAGGCGTATCACGAGGCC</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>TGAGCCTTTCGTTTTATTTGATGC</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>59.68252050089797</v>
-      </c>
-      <c r="J5" t="n">
-        <v>58.83935928832585</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1418</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Cgl1452_ins</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>AATAGGCGTATCACGAGGCCCTTTCTACGGCCCCAAGGTCCAAACGGTGATAGGGATAACAGGGTAATGTACCATTTACGTTGACACCACCTTTCGCGTATGGCATGATAGCGCCGGGAAGAGAGTCAATTCAGGGTGGTGAATATGAATAGTTCGACAAAGATCGCATTGGTAATTACGTTACTCGATGCCATGGGGATTGGCCTTATCATGCCAGTCTTGCCAACGTTATTACGTGAATTTATTGCTTCGGAAGATATCGCTAACCACTTTGGCGTATTGCTTGCACTTTATGCGTTAATGCAGGTTATCTTTGCTCCTTGGCTTGGAAAAATGTCTGACCGATTTGGTCGGCGCCCAGTGCTGTTGTTGTCATTAATAGGCGCATCGCTGGATTACTTATTGCTGGCTTTTTCAAGTGCGCTTTGGATGCTGTATTTAGGCCGTTTGCTTTCAGGGATCACAGGAGCTACTGGGGCTGTCGCGGCATCGGTCATTGCCGATACCACCTCAGCTTCTCAACGCGTGAAGTGGTTCGGTTGGTTAGGGGCAAGTTTTGGGCTTGGTTTAATAGCGGGGCCTATTATTGGTGGTTTTGCAGGAGAGATTTCACCGCATAGTCCCTTTTTTATCGCTGCGTTGCTAAATATTGTCACTTTCCTTGTGGTTATGTTTTGGTTCCGTGAAACCAAAAATACACGTGATAATACAGATACCGAAGTAGGGGTTGAGACGCAATCAAATTCGGTGTACATCACTTTATTTAAAACGATGCCCATTTTGTTGATTATTTATTTTTCAGCGCAATTGATAGGCCAAATTCCCGCAACGGTGTGGGTGCTATTTACCGAAAATCGTTTTGGATGGAATAGCATGATGGTTGGCTTTTCATTAGCGGGTCTTGGTCTTTTACACTCAGTATTCCAAGCCTTTGTGGCAGGAAGAATAGCCACTAAATGGGGCGAAAAAACGGCAGTACTGCTCGGATTTATTGCAGATAGTAGTGCATTTGCCTTTTTAGCGTTTATATCTGAAGGTTGGTTAGTTTTCCCTGTTTTAATTTTATTGGCTGGTGGTGGGATCGCTTTACCTGCATTACAGGGAGTGATGTCTATCCAAACAAAGAGTCATCAGCAAGGTGCTTTACAGGGATTATTGGTGAGCCTTACCAATGCAACCGGTGTTATTGGCCCATTACTGTTTGCTGTTATTTATAATCATTCACTACCAATTTGGGATGGCTGGATTTGGATTATTGGTTTAGCGTTTTACTGTATTATTATCCTGCTATCAATGACCTTCATGTTGACCCCTCAAGCTCAGGGGAGTAAACAGGAGACAAGTGCTTAGTAGGGATAACAGGGTAATGATGGCGCCTCATCCCTGAAGCCAAGGCATCAAATAAAACGAAAGGCTCA</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>-18.06656264433227</v>
-      </c>
-      <c r="E6" t="n">
-        <v>-42.9625693662399</v>
-      </c>
-      <c r="F6" t="n">
-        <v>-7.940638660056891</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>AATAGGCGTATCACGAGGCC</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>TGAGCCTTTCGTTTTATTTGATGC</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>59.68252050089797</v>
-      </c>
-      <c r="J6" t="n">
-        <v>58.83935928832585</v>
-      </c>
-      <c r="K6" t="n">
         <v>1418</v>
       </c>
     </row>

</xml_diff>